<commit_message>
Removed user interface script, updated all other scripts
</commit_message>
<xml_diff>
--- a/src/Data/Inputs.xlsx
+++ b/src/Data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3469CB-5C62-694F-B8FD-866D4E84185F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9023269-DCFF-B242-836E-ABB5DD8EAC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16580" activeTab="8" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
@@ -24,15 +24,15 @@
     <sheet name="README" sheetId="4" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$74,Active!$B$79,Active!$B$81,Active!$B$82</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$80,Active!$B$85,Active!$B$87,Active!$B$88</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'Figure 3'!$B$74,'Figure 3'!$B$79,'Figure 3'!$B$81,'Figure 3'!$B$82</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$85</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$91</definedName>
     <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Figure 3'!$B$85</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$52</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$58</definedName>
     <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Figure 3'!$F$52</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$53</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$59</definedName>
     <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Figure 3'!$F$53</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
@@ -40,7 +40,7 @@
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$51</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$57</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">'Figure 3'!$F$51</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">2</definedName>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="76">
   <si>
     <t>Sample Name</t>
   </si>
@@ -253,6 +253,63 @@
   </si>
   <si>
     <t>at/g</t>
+  </si>
+  <si>
+    <t>Nuclide</t>
+  </si>
+  <si>
+    <t>Atmospheric conversion</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>Plate</t>
+  </si>
+  <si>
+    <t>Nuclide-Mineral</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>3He in qtz</t>
+  </si>
+  <si>
+    <t>3He in pyx</t>
+  </si>
+  <si>
+    <t>3He in ol</t>
+  </si>
+  <si>
+    <t>21Ne in qtz</t>
+  </si>
+  <si>
+    <t>ERA40</t>
+  </si>
+  <si>
+    <t>Standard atmosphere</t>
+  </si>
+  <si>
+    <t>time in Ma</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>ANT</t>
   </si>
 </sst>
 </file>
@@ -351,7 +408,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -393,6 +450,7 @@
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -708,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,9 +785,10 @@
     <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -760,348 +819,791 @@
       <c r="K1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2">
-        <v>75</v>
-      </c>
-      <c r="C2">
-        <v>40</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3">
-        <v>75</v>
-      </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4">
-        <v>75</v>
-      </c>
-      <c r="C4">
-        <v>40</v>
-      </c>
-      <c r="D4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5">
-        <v>75</v>
-      </c>
-      <c r="C5">
-        <v>40</v>
-      </c>
-      <c r="D5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6">
-        <v>75</v>
-      </c>
-      <c r="C6">
-        <v>40</v>
-      </c>
-      <c r="D6">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7">
-        <v>75</v>
-      </c>
-      <c r="C7">
-        <v>40</v>
-      </c>
-      <c r="D7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8">
-        <v>75</v>
-      </c>
-      <c r="C8">
-        <v>40</v>
-      </c>
-      <c r="D8">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9">
-        <v>75</v>
-      </c>
-      <c r="C9">
-        <v>40</v>
-      </c>
-      <c r="D9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10">
-        <v>75</v>
-      </c>
-      <c r="C10">
-        <v>40</v>
-      </c>
-      <c r="D10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11">
-        <v>75</v>
-      </c>
-      <c r="C11">
-        <v>40</v>
-      </c>
-      <c r="D11">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>78</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>78</v>
-      </c>
-      <c r="D13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>78</v>
-      </c>
-      <c r="D14">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>78</v>
-      </c>
-      <c r="D15">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>78</v>
-      </c>
-      <c r="D16">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>78</v>
-      </c>
-      <c r="D17">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>78</v>
-      </c>
-      <c r="D18">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>78</v>
-      </c>
-      <c r="D19">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>78</v>
-      </c>
-      <c r="D20">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>78</v>
-      </c>
-      <c r="D21">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="10"/>
-      <c r="E22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
-      <c r="E23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="10"/>
-      <c r="E24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="9"/>
-      <c r="E25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="9"/>
-      <c r="E26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="9"/>
-      <c r="E27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="9"/>
+      <c r="M1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9">
+        <v>-19.578942000000001</v>
+      </c>
+      <c r="C2" s="9">
+        <v>-69.872967000000003</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1172</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1">
+        <f>65.91*10^7</f>
+        <v>659100000</v>
+      </c>
+      <c r="K2" s="1">
+        <f>1.2*10^7</f>
+        <v>12000000</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>25</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="10">
+        <v>-19.340944</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-69.727999999999994</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1607</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2">
+        <f>74.48*10^7</f>
+        <v>744800000</v>
+      </c>
+      <c r="K3" s="2">
+        <f>2.33*10^7</f>
+        <v>23300000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="10">
+        <v>-19.340944</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-69.727999999999994</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1607</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2">
+        <f>91.1*10^7</f>
+        <v>911000000</v>
+      </c>
+      <c r="K4" s="2">
+        <f>1.3*10^7</f>
+        <v>13000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="10">
+        <v>-19.340944</v>
+      </c>
+      <c r="C5" s="10">
+        <v>-69.727999999999994</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1607</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2">
+        <f>167.12*10^7</f>
+        <v>1671200000</v>
+      </c>
+      <c r="K5" s="2">
+        <f>3.65*10^7</f>
+        <v>36500000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10">
+        <v>-19.336722000000002</v>
+      </c>
+      <c r="C6" s="10">
+        <v>-69.729611000000006</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1604</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2">
+        <f>104.68*10^7</f>
+        <v>1046800000.0000001</v>
+      </c>
+      <c r="K6" s="2">
+        <f>2.24*10^7</f>
+        <v>22400000.000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9">
+        <v>-18.886583000000002</v>
+      </c>
+      <c r="C7" s="9">
+        <v>-69.699055999999999</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2282</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2">
+        <f>269.89*10^7</f>
+        <v>2698900000</v>
+      </c>
+      <c r="K7" s="7">
+        <f>4.73*10^7</f>
+        <v>47300000.000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="9">
+        <v>-18.886583000000002</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-69.699055999999999</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2282</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2">
+        <f>246.53*10^7</f>
+        <v>2465300000</v>
+      </c>
+      <c r="K8" s="7">
+        <f>4.29*10^7</f>
+        <v>42900000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9">
+        <v>-18.905639000000001</v>
+      </c>
+      <c r="C9" s="9">
+        <v>-69.954583</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1443</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2">
+        <f>141.41*10^7</f>
+        <v>1414100000</v>
+      </c>
+      <c r="K9" s="7">
+        <f>2.52*10^7</f>
+        <v>25200000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9">
+        <v>-18.905639000000001</v>
+      </c>
+      <c r="C10" s="9">
+        <v>-69.954583</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1443</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2">
+        <f>164.8*10^7</f>
+        <v>1648000000</v>
+      </c>
+      <c r="K10" s="7">
+        <f>2.84*10^7</f>
+        <v>28400000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="9">
+        <v>-18.852694</v>
+      </c>
+      <c r="C11" s="9">
+        <v>-69.657167000000001</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2550</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2">
+        <f>235*10^7</f>
+        <v>2350000000</v>
+      </c>
+      <c r="K11" s="7">
+        <f>4.04*10^7</f>
+        <v>40400000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9">
+        <v>-20.704083000000001</v>
+      </c>
+      <c r="C12" s="9">
+        <v>-69.420833000000002</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1084</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2">
+        <f>90.19*10^7</f>
+        <v>901900000</v>
+      </c>
+      <c r="K12" s="7">
+        <f>1.97*10^7</f>
+        <v>19700000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="11">
+        <v>-19.786306</v>
+      </c>
+      <c r="C13" s="11">
+        <v>-69.682000000000002</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1289</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2">
+        <f>107.8*10^7</f>
+        <v>1078000000</v>
+      </c>
+      <c r="K13" s="2">
+        <f>2.77*10^7</f>
+        <v>27700000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="10">
+        <v>-19.786306</v>
+      </c>
+      <c r="C14" s="10">
+        <v>-69.682000000000002</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1289</v>
+      </c>
+      <c r="E14" s="1">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2">
+        <f>102.49*10^7</f>
+        <v>1024900000</v>
+      </c>
+      <c r="K14" s="2">
+        <f>2.48*10^7</f>
+        <v>24800000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="10">
+        <v>-19.786306</v>
+      </c>
+      <c r="C15" s="10">
+        <v>-69.682000000000002</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1289</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="8">
+        <f>298.96*10^7</f>
+        <v>2989600000</v>
+      </c>
+      <c r="K15" s="2">
+        <f>3.2*10^7</f>
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="10">
+        <v>-19.397832999999999</v>
+      </c>
+      <c r="C16" s="10">
+        <v>-69.880306000000004</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1256</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="2">
+        <f>194.23*10^7</f>
+        <v>1942300000</v>
+      </c>
+      <c r="K16" s="2">
+        <f>4.67*10^7</f>
+        <v>46700000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="10">
+        <v>-19.397832999999999</v>
+      </c>
+      <c r="C17" s="10">
+        <v>-69.880306000000004</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1256</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2.74</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2">
+        <f>310.26*10^7</f>
+        <v>3102600000</v>
+      </c>
+      <c r="K17" s="2">
+        <f>8.23*10^7</f>
+        <v>82300000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="10">
+        <v>-19.397832999999999</v>
+      </c>
+      <c r="C18" s="10">
+        <v>-69.880306000000004</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1256</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="2">
+        <f>269.16*10^7</f>
+        <v>2691600000.0000005</v>
+      </c>
+      <c r="K18" s="2">
+        <f>6.18*10^7</f>
+        <v>61800000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="9">
+        <v>-19.522110999999999</v>
+      </c>
+      <c r="C19" s="9">
+        <v>-69.808333000000005</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1312</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="13">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="2">
+        <f>277.15*10^7</f>
+        <v>2771500000</v>
+      </c>
+      <c r="K19" s="7">
+        <f>5.2*10^7</f>
+        <v>52000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="9">
+        <v>-19.522110999999999</v>
+      </c>
+      <c r="C20" s="9">
+        <v>-69.808333000000005</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1312</v>
+      </c>
+      <c r="E20" s="1">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2">
+        <f>65.4*10^7</f>
+        <v>654000000</v>
+      </c>
+      <c r="K20" s="7">
+        <f>1.5*10^7</f>
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="12">
+        <v>-18.503527999999999</v>
+      </c>
+      <c r="C21" s="12">
+        <v>-70.143305999999995</v>
+      </c>
+      <c r="D21" s="12">
+        <v>771</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="2">
+        <f>41.29*10^7</f>
+        <v>412900000</v>
+      </c>
+      <c r="K21" s="7">
+        <f>0.72*10^7</f>
+        <v>7200000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2145,10 +2647,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923D42B9-7A86-1345-AADD-F9A6DEC8D2BA}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD21"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2210,7 +2712,7 @@
         <v>40</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2224,7 +2726,7 @@
         <v>40</v>
       </c>
       <c r="D4">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2238,7 +2740,7 @@
         <v>40</v>
       </c>
       <c r="D5">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2252,7 +2754,7 @@
         <v>40</v>
       </c>
       <c r="D6">
-        <v>1500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2266,7 +2768,7 @@
         <v>40</v>
       </c>
       <c r="D7">
-        <v>2000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -2280,7 +2782,7 @@
         <v>40</v>
       </c>
       <c r="D8">
-        <v>2500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -2294,7 +2796,7 @@
         <v>40</v>
       </c>
       <c r="D9">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -2322,108 +2824,108 @@
         <v>40</v>
       </c>
       <c r="D11">
-        <v>5000</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C12">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C13">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D13">
-        <v>100</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C14">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D14">
-        <v>500</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C15">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D15">
-        <v>1000</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C16">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C17">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D17">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C18">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D18">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -2434,10 +2936,10 @@
         <v>78</v>
       </c>
       <c r="D19">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2448,10 +2950,10 @@
         <v>78</v>
       </c>
       <c r="D20">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2462,8 +2964,228 @@
         <v>78</v>
       </c>
       <c r="D21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>78</v>
+      </c>
+      <c r="D22">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>78</v>
+      </c>
+      <c r="D23">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>78</v>
+      </c>
+      <c r="D24">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>78</v>
+      </c>
+      <c r="D25">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>78</v>
+      </c>
+      <c r="D26">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>78</v>
+      </c>
+      <c r="D27">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>78</v>
+      </c>
+      <c r="D28">
+        <v>4500</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>78</v>
+      </c>
+      <c r="D29">
         <v>5000</v>
       </c>
+      <c r="E29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>78</v>
+      </c>
+      <c r="D30">
+        <v>5500</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>78</v>
+      </c>
+      <c r="D31">
+        <v>6000</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>78</v>
+      </c>
+      <c r="D32">
+        <v>6500</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>78</v>
+      </c>
+      <c r="D33">
+        <v>7000</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>78</v>
+      </c>
+      <c r="D34">
+        <v>7500</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>78</v>
+      </c>
+      <c r="D35">
+        <v>8000</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3625,10 +4347,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3642,9 +4364,11 @@
     <col min="8" max="8" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3675,8 +4399,23 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -3707,8 +4446,23 @@
       <c r="J2" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L2" s="15">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3721,8 +4475,17 @@
       <c r="H3" s="13"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3733,8 +4496,14 @@
       <c r="H4" s="13"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3745,8 +4514,14 @@
       <c r="H5" s="13"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3757,8 +4532,11 @@
       <c r="H6" s="13"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3769,8 +4547,11 @@
       <c r="H7" s="13"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3781,8 +4562,11 @@
       <c r="H8" s="13"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3793,8 +4577,11 @@
       <c r="H9" s="13"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3806,7 +4593,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -3818,7 +4605,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -3829,8 +4616,23 @@
       <c r="H12" s="13"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N12" t="s">
+        <v>59</v>
+      </c>
+      <c r="O12" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -3841,8 +4643,23 @@
       <c r="H13" s="13"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L13" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N13" t="s">
+        <v>70</v>
+      </c>
+      <c r="O13" t="s">
+        <v>70</v>
+      </c>
+      <c r="P13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -3853,8 +4670,17 @@
       <c r="H14" s="13"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -3865,8 +4691,14 @@
       <c r="H15" s="13"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>66</v>
+      </c>
+      <c r="P15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -3877,8 +4709,14 @@
       <c r="H16" s="13"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3889,8 +4727,11 @@
       <c r="H17" s="13"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3901,6 +4742,19 @@
       <c r="H18" s="13"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
+      <c r="P18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P20" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed comments in MCADAM script
</commit_message>
<xml_diff>
--- a/src/Data/Inputs.xlsx
+++ b/src/Data/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06A3DAC-BF05-404B-AA35-2993B625B4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2437C8A7-EC69-9C44-825A-4DB35AB7464E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="78">
   <si>
     <t>Sample Name</t>
   </si>
@@ -775,7 +775,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,317 +845,315 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9">
+        <v>90</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1">
+        <f>65.91*10^7</f>
+        <v>659100000</v>
+      </c>
+      <c r="K2" s="1">
+        <f>1.2*10^7</f>
+        <v>12000000</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0.25</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B3" s="10">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C3" s="10">
-        <v>-106</v>
+        <v>0</v>
       </c>
       <c r="D3" s="10">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="1">
-        <v>15</v>
-      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1"/>
       <c r="J3" s="2">
-        <v>2380000</v>
+        <f>74.48*10^7</f>
+        <v>744800000</v>
       </c>
       <c r="K3" s="2">
-        <v>56000</v>
-      </c>
-      <c r="L3">
-        <v>15</v>
+        <f>2.33*10^7</f>
+        <v>23300000</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B4" s="10">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C4" s="10">
-        <v>-106</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="E4" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="1">
-        <v>15</v>
-      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1"/>
       <c r="J4" s="2">
-        <v>2630000</v>
-      </c>
-      <c r="K4" s="7">
-        <v>59000</v>
-      </c>
-      <c r="L4">
-        <v>15</v>
+        <f>91.1*10^7</f>
+        <v>911000000</v>
+      </c>
+      <c r="K4" s="2">
+        <f>1.3*10^7</f>
+        <v>13000000</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>41</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="10">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C5" s="10">
-        <v>-106</v>
+        <v>0</v>
       </c>
       <c r="D5" s="10">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="E5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="1">
-        <v>15</v>
-      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1"/>
       <c r="J5" s="2">
-        <v>2750000</v>
-      </c>
-      <c r="K5" s="7">
-        <v>57000</v>
-      </c>
-      <c r="L5">
-        <v>15</v>
+        <f>167.12*10^7</f>
+        <v>1671200000</v>
+      </c>
+      <c r="K5" s="2">
+        <f>3.65*10^7</f>
+        <v>36500000</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="10">
-        <v>38</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D6" s="10">
-        <v>2500</v>
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="9">
+        <v>90</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2000</v>
       </c>
       <c r="E6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="1">
-        <v>35</v>
-      </c>
-      <c r="J6" s="2">
-        <v>330000</v>
-      </c>
-      <c r="K6" s="7">
-        <v>550000</v>
-      </c>
-      <c r="L6">
-        <v>35</v>
+      <c r="H6" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>42</v>
+      <c r="A7" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B7" s="10">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C7" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2500</v>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2000</v>
       </c>
       <c r="E7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="1">
-        <v>45</v>
-      </c>
-      <c r="J7" s="2">
-        <v>730000</v>
-      </c>
-      <c r="K7" s="7">
-        <v>540000</v>
-      </c>
-      <c r="L7">
-        <v>45</v>
+      <c r="H7" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>43</v>
+      <c r="A8" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B8" s="10">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C8" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D8" s="10">
-        <v>2500</v>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4000</v>
       </c>
       <c r="E8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="1">
-        <v>35</v>
-      </c>
-      <c r="J8" s="2">
-        <v>340000</v>
-      </c>
-      <c r="K8" s="7">
-        <v>600000</v>
-      </c>
-      <c r="L8">
-        <v>35</v>
+      <c r="H8" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>40</v>
+      <c r="A9" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B9" s="10">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C9" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D9" s="10">
-        <v>2500</v>
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4000</v>
       </c>
       <c r="E9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="1">
-        <v>55</v>
-      </c>
-      <c r="J9" s="2">
-        <v>590000</v>
-      </c>
-      <c r="K9" s="7">
-        <v>560000</v>
-      </c>
-      <c r="L9">
-        <v>55</v>
+      <c r="H9" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="7"/>
+      <c r="A10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="9">
+        <v>90</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="7"/>
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
@@ -2387,7 +2385,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3037,10 +3035,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24694F2A-853A-E44C-A507-6368D3EEDD55}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD8"/>
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3337,10 +3335,6 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed MCADAM to medians
</commit_message>
<xml_diff>
--- a/src/Data/Inputs.xlsx
+++ b/src/Data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B410DEF6-CF22-BB46-BF43-29F33A132322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B58E022-79D4-5241-B3DF-90EE9284BF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="8" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="137">
   <si>
     <t>Sample Name</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t>1 = Yes (see Mijjum et al. (2023) for discussion on this parameter)</t>
+  </si>
+  <si>
+    <t>Topographic shielding correction</t>
   </si>
 </sst>
 </file>
@@ -840,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1003,9 +1006,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,17 +1027,47 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1051,69 +1081,8 @@
     <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1430,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1457,685 +1426,1000 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="67" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="67" t="s">
+    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="67" t="s">
+      <c r="F1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="O1" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="66" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="87" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="87">
+      <c r="B2" s="15">
         <v>-20.101167</v>
       </c>
-      <c r="C2" s="87">
+      <c r="C2" s="15">
         <v>-69.491221999999993</v>
       </c>
-      <c r="D2" s="87">
+      <c r="D2" s="15">
         <v>1380</v>
       </c>
-      <c r="E2" s="87">
-        <v>5</v>
-      </c>
-      <c r="F2" s="89">
+      <c r="E2" s="15">
+        <v>5</v>
+      </c>
+      <c r="F2" s="26">
         <v>3.2</v>
       </c>
-      <c r="G2" s="87">
-        <v>1</v>
-      </c>
-      <c r="H2" s="87">
-        <v>0</v>
-      </c>
-      <c r="I2" s="88">
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="27">
         <f>3.23*10^7</f>
         <v>32300000</v>
       </c>
-      <c r="J2" s="88">
+      <c r="J2" s="27">
         <v>4900000</v>
       </c>
-      <c r="L2" s="90">
+      <c r="L2">
         <v>2</v>
       </c>
-      <c r="M2" s="90">
-        <v>1</v>
-      </c>
-      <c r="N2" s="90">
-        <v>0</v>
-      </c>
-      <c r="O2" s="90">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
         <v>20</v>
       </c>
-      <c r="P2" s="90">
+      <c r="P2">
         <v>2</v>
       </c>
-      <c r="R2" s="90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="91" t="s">
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="91">
+      <c r="B3" s="14">
         <v>-20.101167</v>
       </c>
-      <c r="C3" s="91">
+      <c r="C3" s="14">
         <v>-69.491221999999993</v>
       </c>
-      <c r="D3" s="91">
+      <c r="D3" s="14">
         <v>1380</v>
       </c>
-      <c r="E3" s="91">
-        <v>5</v>
-      </c>
-      <c r="F3" s="89">
+      <c r="E3" s="14">
+        <v>5</v>
+      </c>
+      <c r="F3" s="22">
         <v>3.2</v>
       </c>
-      <c r="G3" s="87">
-        <v>1</v>
-      </c>
-      <c r="H3" s="87">
-        <v>0</v>
-      </c>
-      <c r="I3" s="92">
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="25">
         <f>25.9*10^7</f>
         <v>259000000</v>
       </c>
-      <c r="J3" s="92">
+      <c r="J3" s="25">
         <v>8800000</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="87" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="87">
+      <c r="B4" s="13">
         <v>-19.578942000000001</v>
       </c>
-      <c r="C4" s="87">
+      <c r="C4" s="13">
         <v>-69.872967000000003</v>
       </c>
-      <c r="D4" s="87">
+      <c r="D4" s="13">
         <v>1172</v>
       </c>
-      <c r="E4" s="87">
-        <v>5</v>
-      </c>
-      <c r="F4" s="89">
+      <c r="E4" s="13">
+        <v>5</v>
+      </c>
+      <c r="F4" s="22">
         <v>2.89</v>
       </c>
-      <c r="G4" s="87">
-        <v>1</v>
-      </c>
-      <c r="H4" s="87">
-        <v>0</v>
-      </c>
-      <c r="I4" s="88">
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="23">
         <f>65.91*10^7</f>
         <v>659100000</v>
       </c>
-      <c r="J4" s="88">
+      <c r="J4" s="23">
         <v>12000000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="87" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="87">
+      <c r="B5" s="13">
         <v>-19.578942000000001</v>
       </c>
-      <c r="C5" s="87">
+      <c r="C5" s="13">
         <v>-69.872967000000003</v>
       </c>
-      <c r="D5" s="87">
+      <c r="D5" s="13">
         <v>1172</v>
       </c>
-      <c r="E5" s="87">
-        <v>5</v>
-      </c>
-      <c r="F5" s="89">
+      <c r="E5" s="15">
+        <v>5</v>
+      </c>
+      <c r="F5" s="22">
         <v>2.89</v>
       </c>
-      <c r="G5" s="87">
-        <v>1</v>
-      </c>
-      <c r="H5" s="87">
-        <v>0</v>
-      </c>
-      <c r="I5" s="88">
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="23">
         <f>32.2*10^7</f>
         <v>322000000</v>
       </c>
-      <c r="J5" s="88">
+      <c r="J5" s="23">
         <v>7000000</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="91" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="91">
+      <c r="B6" s="14">
         <v>-19.987110999999999</v>
       </c>
-      <c r="C6" s="91">
+      <c r="C6" s="14">
         <v>-69.433610999999999</v>
       </c>
-      <c r="D6" s="91">
+      <c r="D6" s="14">
         <v>1943</v>
       </c>
-      <c r="E6" s="91">
-        <v>5</v>
-      </c>
-      <c r="F6" s="89">
+      <c r="E6" s="14">
+        <v>5</v>
+      </c>
+      <c r="F6" s="22">
         <v>2.89</v>
       </c>
-      <c r="G6" s="87">
-        <v>1</v>
-      </c>
-      <c r="H6" s="87">
-        <v>0</v>
-      </c>
-      <c r="I6" s="92">
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="25">
         <f>63.88*10^7</f>
         <v>638800000</v>
       </c>
-      <c r="J6" s="92">
+      <c r="J6" s="25">
         <v>25700000</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="91" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="91">
+      <c r="B7" s="14">
         <v>-19.340944</v>
       </c>
-      <c r="C7" s="91">
+      <c r="C7" s="14">
         <v>-69.727999999999994</v>
       </c>
-      <c r="D7" s="91">
+      <c r="D7" s="14">
         <v>1607</v>
       </c>
-      <c r="E7" s="87">
-        <v>5</v>
-      </c>
-      <c r="F7" s="89">
+      <c r="E7" s="13">
+        <v>5</v>
+      </c>
+      <c r="F7" s="22">
         <v>2.89</v>
       </c>
-      <c r="G7" s="87">
-        <v>1</v>
-      </c>
-      <c r="H7" s="87">
-        <v>0</v>
-      </c>
-      <c r="I7" s="92">
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="25">
         <f>74.48*10^7</f>
         <v>744800000</v>
       </c>
-      <c r="J7" s="92">
+      <c r="J7" s="25">
         <v>23300000</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="91" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="91">
+      <c r="B8" s="14">
         <v>-19.340944</v>
       </c>
-      <c r="C8" s="91">
+      <c r="C8" s="14">
         <v>-69.727999999999994</v>
       </c>
-      <c r="D8" s="91">
+      <c r="D8" s="14">
         <v>1607</v>
       </c>
-      <c r="E8" s="87">
-        <v>5</v>
-      </c>
-      <c r="F8" s="89">
+      <c r="E8" s="15">
+        <v>5</v>
+      </c>
+      <c r="F8" s="22">
         <v>2.89</v>
       </c>
-      <c r="G8" s="87">
-        <v>1</v>
-      </c>
-      <c r="H8" s="87">
-        <v>0</v>
-      </c>
-      <c r="I8" s="92">
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25">
         <f>91.1*10^7</f>
         <v>911000000</v>
       </c>
-      <c r="J8" s="92">
+      <c r="J8" s="25">
         <v>13000000</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="91" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="91">
+      <c r="B9" s="14">
         <v>-19.340944</v>
       </c>
-      <c r="C9" s="91">
+      <c r="C9" s="14">
         <v>-69.727999999999994</v>
       </c>
-      <c r="D9" s="91">
+      <c r="D9" s="14">
         <v>1607</v>
       </c>
-      <c r="E9" s="91">
-        <v>5</v>
-      </c>
-      <c r="F9" s="89">
+      <c r="E9" s="14">
+        <v>5</v>
+      </c>
+      <c r="F9" s="22">
         <v>2.89</v>
       </c>
-      <c r="G9" s="87">
-        <v>1</v>
-      </c>
-      <c r="H9" s="87">
-        <v>0</v>
-      </c>
-      <c r="I9" s="92">
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0</v>
+      </c>
+      <c r="I9" s="25">
         <f>167.12*10^7</f>
         <v>1671200000</v>
       </c>
-      <c r="J9" s="92">
+      <c r="J9" s="25">
         <v>36500000</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="91" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="91">
+      <c r="B10" s="14">
         <v>-19.336722000000002</v>
       </c>
-      <c r="C10" s="91">
+      <c r="C10" s="14">
         <v>-69.729611000000006</v>
       </c>
-      <c r="D10" s="91">
+      <c r="D10" s="14">
         <v>1604</v>
       </c>
-      <c r="E10" s="87">
-        <v>5</v>
-      </c>
-      <c r="F10" s="89">
+      <c r="E10" s="13">
+        <v>5</v>
+      </c>
+      <c r="F10" s="22">
         <v>2.89</v>
       </c>
-      <c r="G10" s="87">
-        <v>1</v>
-      </c>
-      <c r="H10" s="87">
-        <v>0</v>
-      </c>
-      <c r="I10" s="92">
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="25">
         <f>24.27*10^7</f>
         <v>242700000</v>
       </c>
-      <c r="J10" s="92">
+      <c r="J10" s="25">
         <v>10500000</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="91" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="91">
+      <c r="B11" s="14">
         <v>-19.336722000000002</v>
       </c>
-      <c r="C11" s="91">
+      <c r="C11" s="14">
         <v>-69.729611000000006</v>
       </c>
-      <c r="D11" s="91">
+      <c r="D11" s="14">
         <v>1604</v>
       </c>
-      <c r="E11" s="87">
-        <v>5</v>
-      </c>
-      <c r="F11" s="89">
+      <c r="E11" s="15">
+        <v>5</v>
+      </c>
+      <c r="F11" s="22">
         <v>2.89</v>
       </c>
-      <c r="G11" s="87">
-        <v>1</v>
-      </c>
-      <c r="H11" s="87">
-        <v>0</v>
-      </c>
-      <c r="I11" s="92">
+      <c r="G11" s="13">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="I11" s="25">
         <f>31.18*10^7</f>
         <v>311800000</v>
       </c>
-      <c r="J11" s="92">
+      <c r="J11" s="25">
         <v>11900000</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="91" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="91">
+      <c r="B12" s="14">
         <v>-19.336722000000002</v>
       </c>
-      <c r="C12" s="91">
+      <c r="C12" s="14">
         <v>-69.729611000000006</v>
       </c>
-      <c r="D12" s="91">
+      <c r="D12" s="14">
         <v>1604</v>
       </c>
-      <c r="E12" s="91">
-        <v>5</v>
-      </c>
-      <c r="F12" s="89">
+      <c r="E12" s="14">
+        <v>5</v>
+      </c>
+      <c r="F12" s="22">
         <v>2.89</v>
       </c>
-      <c r="G12" s="87">
-        <v>1</v>
-      </c>
-      <c r="H12" s="87">
-        <v>0</v>
-      </c>
-      <c r="I12" s="92">
+      <c r="G12" s="13">
+        <v>1</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="25">
         <f>104.68*10^7</f>
         <v>1046800000.0000001</v>
       </c>
-      <c r="J12" s="92">
+      <c r="J12" s="25">
         <v>22400000.000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="87" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="87">
+      <c r="B13" s="16">
         <v>-18.886583000000002</v>
       </c>
-      <c r="C13" s="87">
+      <c r="C13" s="16">
         <v>-69.699055999999999</v>
       </c>
-      <c r="D13" s="87">
+      <c r="D13" s="16">
         <v>2282</v>
       </c>
-      <c r="E13" s="87">
-        <v>5</v>
-      </c>
-      <c r="F13" s="89">
+      <c r="E13" s="13">
+        <v>5</v>
+      </c>
+      <c r="F13" s="22">
         <v>2.89</v>
       </c>
-      <c r="G13" s="87">
-        <v>1</v>
-      </c>
-      <c r="H13" s="87">
-        <v>0</v>
-      </c>
-      <c r="I13" s="88">
+      <c r="G13" s="13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="28">
         <f>269.89*10^7</f>
         <v>2698900000</v>
       </c>
-      <c r="J13" s="88">
+      <c r="J13" s="28">
         <v>47300000.000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="87" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="87">
+      <c r="B14" s="16">
         <v>-18.886583000000002</v>
       </c>
-      <c r="C14" s="87">
+      <c r="C14" s="16">
         <v>-69.699055999999999</v>
       </c>
-      <c r="D14" s="87">
+      <c r="D14" s="16">
         <v>2282</v>
       </c>
-      <c r="E14" s="87">
-        <v>5</v>
-      </c>
-      <c r="F14" s="89">
+      <c r="E14" s="15">
+        <v>5</v>
+      </c>
+      <c r="F14" s="22">
         <v>2.89</v>
       </c>
-      <c r="G14" s="87">
-        <v>1</v>
-      </c>
-      <c r="H14" s="87">
-        <v>0</v>
-      </c>
-      <c r="I14" s="88">
+      <c r="G14" s="13">
+        <v>1</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="28">
         <f>246.53*10^7</f>
         <v>2465300000</v>
       </c>
-      <c r="J14" s="88">
+      <c r="J14" s="28">
         <v>42900000</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="90" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="91"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="93"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="91"/>
-    </row>
-    <row r="16" spans="1:18" s="90" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="87"/>
-      <c r="B17" s="87"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
-    </row>
-    <row r="18" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="87"/>
-      <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="88"/>
-    </row>
-    <row r="19" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="91"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="J19" s="92"/>
-      <c r="K19" s="92"/>
-    </row>
-    <row r="20" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="91"/>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="87"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-    </row>
-    <row r="21" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="95"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="87"/>
-      <c r="H21" s="87"/>
-      <c r="J21" s="96"/>
-      <c r="K21" s="92"/>
-    </row>
-    <row r="22" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="91"/>
-      <c r="B22" s="91"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="92"/>
-    </row>
-    <row r="23" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="91"/>
-      <c r="B23" s="91"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="92"/>
-    </row>
-    <row r="24" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="91"/>
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="91"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-    </row>
-    <row r="25" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="87"/>
-      <c r="B25" s="87"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="J25" s="88"/>
-      <c r="K25" s="88"/>
-    </row>
-    <row r="26" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="87"/>
-      <c r="B26" s="87"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-    </row>
-    <row r="27" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="97"/>
-      <c r="B27" s="87"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="88"/>
-    </row>
-    <row r="28" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="87"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="88"/>
-    </row>
-    <row r="29" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="87"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="J29" s="88"/>
-      <c r="K29" s="88"/>
-    </row>
-    <row r="30" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E30" s="89"/>
-      <c r="H30" s="89"/>
-      <c r="I30" s="89"/>
-    </row>
-    <row r="31" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E31" s="89"/>
-      <c r="H31" s="89"/>
-      <c r="I31" s="89"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="16">
+        <v>-18.905639000000001</v>
+      </c>
+      <c r="C15" s="16">
+        <v>-69.954583</v>
+      </c>
+      <c r="D15" s="16">
+        <v>1443</v>
+      </c>
+      <c r="E15" s="14">
+        <v>5</v>
+      </c>
+      <c r="F15" s="22">
+        <v>2.89</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
+      <c r="I15" s="28">
+        <v>1414100000</v>
+      </c>
+      <c r="J15" s="28">
+        <v>25200000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="16">
+        <v>-18.905639000000001</v>
+      </c>
+      <c r="C16" s="16">
+        <v>-69.954583</v>
+      </c>
+      <c r="D16" s="16">
+        <v>1443</v>
+      </c>
+      <c r="E16" s="13">
+        <v>5</v>
+      </c>
+      <c r="F16" s="22">
+        <v>2.89</v>
+      </c>
+      <c r="G16" s="13">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13">
+        <v>0</v>
+      </c>
+      <c r="I16" s="28">
+        <v>1648000000</v>
+      </c>
+      <c r="J16" s="28">
+        <v>28400000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="16">
+        <v>-18.852694</v>
+      </c>
+      <c r="C17" s="16">
+        <v>-69.657167000000001</v>
+      </c>
+      <c r="D17" s="16">
+        <v>2550</v>
+      </c>
+      <c r="E17" s="15">
+        <v>5</v>
+      </c>
+      <c r="F17" s="22">
+        <v>2.89</v>
+      </c>
+      <c r="G17" s="13">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0</v>
+      </c>
+      <c r="I17" s="28">
+        <v>2350000000</v>
+      </c>
+      <c r="J17" s="28">
+        <v>40400000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="16">
+        <v>-20.704083000000001</v>
+      </c>
+      <c r="C18" s="16">
+        <v>-69.420833000000002</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1084</v>
+      </c>
+      <c r="E18" s="14">
+        <v>5</v>
+      </c>
+      <c r="F18" s="22">
+        <v>2.89</v>
+      </c>
+      <c r="G18" s="13">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13">
+        <v>0</v>
+      </c>
+      <c r="I18" s="28">
+        <v>901900000</v>
+      </c>
+      <c r="J18" s="28">
+        <v>19700000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="17">
+        <v>-19.786306</v>
+      </c>
+      <c r="C19" s="17">
+        <v>-69.682000000000002</v>
+      </c>
+      <c r="D19" s="17">
+        <v>1289</v>
+      </c>
+      <c r="E19" s="13">
+        <v>5</v>
+      </c>
+      <c r="F19" s="26">
+        <v>2.89</v>
+      </c>
+      <c r="G19" s="13">
+        <v>1</v>
+      </c>
+      <c r="H19" s="13">
+        <v>0</v>
+      </c>
+      <c r="I19" s="29">
+        <v>1078000000</v>
+      </c>
+      <c r="J19" s="29">
+        <v>27700000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="14">
+        <v>-19.786306</v>
+      </c>
+      <c r="C20" s="14">
+        <v>-69.682000000000002</v>
+      </c>
+      <c r="D20" s="14">
+        <v>1289</v>
+      </c>
+      <c r="E20" s="15">
+        <v>5</v>
+      </c>
+      <c r="F20" s="22">
+        <v>2.89</v>
+      </c>
+      <c r="G20" s="13">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13">
+        <v>0</v>
+      </c>
+      <c r="I20" s="25">
+        <v>1024900000</v>
+      </c>
+      <c r="J20" s="25">
+        <v>24800000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="14">
+        <v>-19.786306</v>
+      </c>
+      <c r="C21" s="14">
+        <v>-69.682000000000002</v>
+      </c>
+      <c r="D21" s="14">
+        <v>1289</v>
+      </c>
+      <c r="E21" s="14">
+        <v>5</v>
+      </c>
+      <c r="F21" s="22">
+        <v>2.89</v>
+      </c>
+      <c r="G21" s="13">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0</v>
+      </c>
+      <c r="I21" s="30">
+        <v>2989600000</v>
+      </c>
+      <c r="J21" s="25">
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="14">
+        <v>-19.397832999999999</v>
+      </c>
+      <c r="C22" s="14">
+        <v>-69.880306000000004</v>
+      </c>
+      <c r="D22" s="14">
+        <v>1256</v>
+      </c>
+      <c r="E22" s="13">
+        <v>5</v>
+      </c>
+      <c r="F22" s="22">
+        <v>2.89</v>
+      </c>
+      <c r="G22" s="13">
+        <v>1</v>
+      </c>
+      <c r="H22" s="13">
+        <v>0</v>
+      </c>
+      <c r="I22" s="25">
+        <v>1942300000</v>
+      </c>
+      <c r="J22" s="25">
+        <v>46700000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="14">
+        <v>-19.397832999999999</v>
+      </c>
+      <c r="C23" s="14">
+        <v>-69.880306000000004</v>
+      </c>
+      <c r="D23" s="14">
+        <v>1256</v>
+      </c>
+      <c r="E23" s="15">
+        <v>5</v>
+      </c>
+      <c r="F23" s="22">
+        <v>2.74</v>
+      </c>
+      <c r="G23" s="13">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13">
+        <v>0</v>
+      </c>
+      <c r="I23" s="25">
+        <v>3102600000</v>
+      </c>
+      <c r="J23" s="25">
+        <v>82300000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="14">
+        <v>-19.397832999999999</v>
+      </c>
+      <c r="C24" s="14">
+        <v>-69.880306000000004</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1256</v>
+      </c>
+      <c r="E24" s="14">
+        <v>5</v>
+      </c>
+      <c r="F24" s="24">
+        <v>2.89</v>
+      </c>
+      <c r="G24" s="13">
+        <v>1</v>
+      </c>
+      <c r="H24" s="13">
+        <v>0</v>
+      </c>
+      <c r="I24" s="25">
+        <v>2691600000.0000005</v>
+      </c>
+      <c r="J24" s="25">
+        <v>61800000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="16">
+        <v>-19.522110999999999</v>
+      </c>
+      <c r="C25" s="16">
+        <v>-69.808333000000005</v>
+      </c>
+      <c r="D25" s="16">
+        <v>1312</v>
+      </c>
+      <c r="E25" s="13">
+        <v>5</v>
+      </c>
+      <c r="F25" s="22">
+        <v>2.89</v>
+      </c>
+      <c r="G25" s="13">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13">
+        <v>0</v>
+      </c>
+      <c r="I25" s="28">
+        <v>2771500000</v>
+      </c>
+      <c r="J25" s="28">
+        <v>52000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="16">
+        <v>-19.522110999999999</v>
+      </c>
+      <c r="C26" s="16">
+        <v>-69.808333000000005</v>
+      </c>
+      <c r="D26" s="16">
+        <v>1312</v>
+      </c>
+      <c r="E26" s="15">
+        <v>5</v>
+      </c>
+      <c r="F26" s="22">
+        <v>2.89</v>
+      </c>
+      <c r="G26" s="13">
+        <v>1</v>
+      </c>
+      <c r="H26" s="13">
+        <v>0</v>
+      </c>
+      <c r="I26" s="28">
+        <v>654000000</v>
+      </c>
+      <c r="J26" s="28">
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="21">
+        <v>-18.503527999999999</v>
+      </c>
+      <c r="C27" s="21">
+        <v>-70.143305999999995</v>
+      </c>
+      <c r="D27" s="21">
+        <v>771</v>
+      </c>
+      <c r="E27" s="14">
+        <v>5</v>
+      </c>
+      <c r="F27" s="31">
+        <v>2.89</v>
+      </c>
+      <c r="G27" s="13">
+        <v>1</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0</v>
+      </c>
+      <c r="I27" s="32">
+        <v>412900000</v>
+      </c>
+      <c r="J27" s="32">
+        <v>7200000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="20">
+        <v>-18.389944</v>
+      </c>
+      <c r="C28" s="20">
+        <v>-70.071805999999995</v>
+      </c>
+      <c r="D28" s="20">
+        <v>1025</v>
+      </c>
+      <c r="E28" s="13">
+        <v>5</v>
+      </c>
+      <c r="F28" s="26">
+        <v>2.89</v>
+      </c>
+      <c r="G28" s="13">
+        <v>1</v>
+      </c>
+      <c r="H28" s="13">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>388000000</v>
+      </c>
+      <c r="J28" s="33">
+        <v>7700000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="21">
+        <v>-18.389944</v>
+      </c>
+      <c r="C29" s="21">
+        <v>-70.071805999999995</v>
+      </c>
+      <c r="D29" s="21">
+        <v>1025</v>
+      </c>
+      <c r="E29" s="15">
+        <v>5</v>
+      </c>
+      <c r="F29" s="31">
+        <v>2.89</v>
+      </c>
+      <c r="G29" s="13">
+        <v>1</v>
+      </c>
+      <c r="H29" s="13">
+        <v>0</v>
+      </c>
+      <c r="I29" s="32">
+        <v>425000000</v>
+      </c>
+      <c r="J29" s="32">
+        <v>9500000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2154,6 +2438,61 @@
       <c r="E35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="12"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="Q49" s="1"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="Q50" s="1"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="Q51" s="1"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="12"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="Q52" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2165,8 +2504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC832A4-C899-574A-A718-CA2E3961F592}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2177,56 +2516,56 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="67" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="67" t="s">
+    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="67" t="s">
+      <c r="F1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="O1" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="66" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4197,7 +4536,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -4226,56 +4565,56 @@
     <col min="19" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="67" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="67" t="s">
+    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="67" t="s">
+      <c r="F1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="O1" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="66" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4301,7 +4640,7 @@
       <c r="G2" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="61" t="s">
+      <c r="H2" s="60" t="s">
         <v>106</v>
       </c>
       <c r="I2" s="56" t="s">
@@ -4314,7 +4653,7 @@
       <c r="L2" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="M2" s="62" t="s">
+      <c r="M2" s="61" t="s">
         <v>118</v>
       </c>
       <c r="N2" s="56" t="s">
@@ -4336,28 +4675,28 @@
     <row r="3" spans="1:18" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="57"/>
       <c r="C3" s="57"/>
-      <c r="H3" s="61"/>
+      <c r="H3" s="60"/>
       <c r="J3" s="58"/>
       <c r="K3" s="58"/>
     </row>
     <row r="4" spans="1:18" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="57"/>
       <c r="C4" s="57"/>
-      <c r="H4" s="61"/>
+      <c r="H4" s="60"/>
       <c r="J4" s="58"/>
       <c r="K4" s="58"/>
     </row>
     <row r="5" spans="1:18" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="57"/>
       <c r="C5" s="57"/>
-      <c r="H5" s="61"/>
+      <c r="H5" s="60"/>
       <c r="J5" s="58"/>
       <c r="K5" s="58"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="H6" s="64"/>
+      <c r="H6" s="63"/>
       <c r="J6" s="59"/>
       <c r="K6" s="59"/>
     </row>
@@ -4365,7 +4704,7 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="H7" s="64"/>
+      <c r="H7" s="63"/>
       <c r="J7" s="59"/>
       <c r="K7" s="59"/>
     </row>
@@ -4373,7 +4712,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="H8" s="64"/>
+      <c r="H8" s="63"/>
       <c r="J8" s="59"/>
       <c r="K8" s="59"/>
     </row>
@@ -4381,7 +4720,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="H9" s="64"/>
+      <c r="H9" s="63"/>
       <c r="J9" s="59"/>
       <c r="K9" s="59"/>
     </row>
@@ -4389,205 +4728,205 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="H10" s="64"/>
+      <c r="H10" s="63"/>
       <c r="I10" s="59"/>
       <c r="J10" s="59"/>
-      <c r="Q10" s="86"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="H11" s="64"/>
+      <c r="H11" s="63"/>
       <c r="I11" s="59"/>
       <c r="J11" s="59"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="H12" s="64"/>
+      <c r="H12" s="63"/>
       <c r="I12" s="59"/>
       <c r="J12" s="59"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="H13" s="64"/>
+      <c r="H13" s="63"/>
       <c r="I13" s="59"/>
       <c r="J13" s="59"/>
-      <c r="L13" s="65"/>
+      <c r="L13" s="64"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-      <c r="H14" s="64"/>
+      <c r="H14" s="63"/>
       <c r="I14" s="59"/>
       <c r="J14" s="59"/>
     </row>
     <row r="15" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="69" t="s">
+      <c r="C15" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="D15" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="68" t="s">
+      <c r="E15" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="F15" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="G15" s="71" t="s">
+      <c r="G15" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="H15" s="74" t="s">
+      <c r="H15" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="I15" s="75" t="s">
+      <c r="I15" s="84" t="s">
         <v>112</v>
       </c>
-      <c r="J15" s="75" t="s">
+      <c r="J15" s="84" t="s">
         <v>112</v>
       </c>
-      <c r="L15" s="71" t="s">
+      <c r="L15" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="M15" s="78" t="s">
+      <c r="M15" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="N15" s="71" t="s">
+      <c r="N15" s="67" t="s">
         <v>122</v>
       </c>
-      <c r="O15" s="78" t="s">
+      <c r="O15" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="P15" s="71" t="s">
+      <c r="P15" s="67" t="s">
         <v>131</v>
       </c>
-      <c r="Q15" s="85" t="s">
+      <c r="Q15" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="R15" s="63" t="s">
+      <c r="R15" s="62" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="72" t="s">
+      <c r="A16" s="79"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="H16" s="74"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="L16" s="76" t="s">
+      <c r="H16" s="83"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="L16" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="M16" s="79" t="s">
+      <c r="M16" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="N16" s="76" t="s">
+      <c r="N16" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="O16" s="82" t="s">
+      <c r="O16" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="P16" s="76" t="s">
+      <c r="P16" s="68" t="s">
         <v>132</v>
       </c>
-      <c r="R16" s="60" t="s">
+      <c r="R16" s="78" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="68"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="L17" s="76" t="s">
+      <c r="A17" s="79"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="84"/>
+      <c r="L17" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="N17" s="80" t="s">
+      <c r="N17" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="83" t="s">
+      <c r="O17" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="76" t="s">
+      <c r="P17" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="R17" s="60"/>
+      <c r="R17" s="78"/>
     </row>
     <row r="18" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="68"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="L18" s="77" t="s">
+      <c r="A18" s="79"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="84"/>
+      <c r="L18" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="N18" s="80"/>
-      <c r="O18" s="83"/>
-      <c r="P18" s="76" t="s">
+      <c r="N18" s="74"/>
+      <c r="O18" s="76"/>
+      <c r="P18" s="68" t="s">
         <v>126</v>
       </c>
-      <c r="R18" s="60"/>
+      <c r="R18" s="78"/>
     </row>
     <row r="19" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="G19" s="73"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="84"/>
-      <c r="P19" s="76" t="s">
+      <c r="G19" s="82"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="84"/>
+      <c r="N19" s="75"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="R19" s="60"/>
+      <c r="R19" s="78"/>
     </row>
     <row r="20" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="P20" s="76" t="s">
+      <c r="P20" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="R20" s="60"/>
+      <c r="R20" s="78"/>
     </row>
     <row r="21" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="P21" s="76" t="s">
+      <c r="P21" s="68" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="P22" s="77" t="s">
+      <c r="P22" s="69" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="O28" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
     <mergeCell ref="J15:J19"/>
     <mergeCell ref="N17:N19"/>
     <mergeCell ref="O17:O19"/>
@@ -4597,10 +4936,6 @@
     <mergeCell ref="G16:G19"/>
     <mergeCell ref="H15:H19"/>
     <mergeCell ref="I15:I19"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4611,61 +4946,61 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" s="67" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="67" t="s">
+    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="67" t="s">
+      <c r="F1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="O1" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="66" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4696,7 +5031,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -4705,10 +5040,16 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="P2">
         <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -4955,7 +5296,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6008,41 +6349,62 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="F1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" s="66" t="s">
         <v>8</v>
+      </c>
+      <c r="L1" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="66" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -6061,20 +6423,23 @@
       <c r="E2" s="9">
         <v>5</v>
       </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
       <c r="M2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="P2">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="Q2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -6135,7 +6500,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6694,67 +7059,87 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC98A15-AE39-4743-9E74-0C5D457F6E10}">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD14"/>
+      <selection activeCell="A2" sqref="A2:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="F1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="N1" t="s">
+      <c r="M1" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="N1" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
+      <c r="O1" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="P1" s="66" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q1" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="66" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>40</v>
       </c>
@@ -6779,30 +7164,36 @@
       <c r="H2" s="13">
         <v>0</v>
       </c>
-      <c r="J2" s="27">
+      <c r="I2" s="27">
         <f>3.23*10^7</f>
         <v>32300000</v>
       </c>
-      <c r="K2" s="27">
+      <c r="J2" s="27">
         <v>4900000</v>
       </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
       <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>20</v>
+      </c>
+      <c r="P2">
         <v>2</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>20</v>
-      </c>
       <c r="Q2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>41</v>
       </c>
@@ -6827,15 +7218,15 @@
       <c r="H3" s="13">
         <v>0</v>
       </c>
-      <c r="J3" s="25">
+      <c r="I3" s="25">
         <f>25.9*10^7</f>
         <v>259000000</v>
       </c>
-      <c r="K3" s="25">
+      <c r="J3" s="25">
         <v>8800000</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
@@ -6860,15 +7251,15 @@
       <c r="H4" s="13">
         <v>0</v>
       </c>
-      <c r="J4" s="23">
+      <c r="I4" s="23">
         <f>65.91*10^7</f>
         <v>659100000</v>
       </c>
-      <c r="K4" s="23">
+      <c r="J4" s="23">
         <v>12000000</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -6893,15 +7284,15 @@
       <c r="H5" s="13">
         <v>0</v>
       </c>
-      <c r="J5" s="23">
+      <c r="I5" s="23">
         <f>32.2*10^7</f>
         <v>322000000</v>
       </c>
-      <c r="K5" s="23">
+      <c r="J5" s="23">
         <v>7000000</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>44</v>
       </c>
@@ -6926,15 +7317,15 @@
       <c r="H6" s="13">
         <v>0</v>
       </c>
-      <c r="J6" s="25">
+      <c r="I6" s="25">
         <f>63.88*10^7</f>
         <v>638800000</v>
       </c>
-      <c r="K6" s="25">
+      <c r="J6" s="25">
         <v>25700000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>45</v>
       </c>
@@ -6959,15 +7350,15 @@
       <c r="H7" s="13">
         <v>0</v>
       </c>
-      <c r="J7" s="25">
+      <c r="I7" s="25">
         <f>74.48*10^7</f>
         <v>744800000</v>
       </c>
-      <c r="K7" s="25">
+      <c r="J7" s="25">
         <v>23300000</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>49</v>
       </c>
@@ -6992,15 +7383,15 @@
       <c r="H8" s="13">
         <v>0</v>
       </c>
-      <c r="J8" s="25">
+      <c r="I8" s="25">
         <f>91.1*10^7</f>
         <v>911000000</v>
       </c>
-      <c r="K8" s="25">
+      <c r="J8" s="25">
         <v>13000000</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>50</v>
       </c>
@@ -7025,15 +7416,15 @@
       <c r="H9" s="13">
         <v>0</v>
       </c>
-      <c r="J9" s="25">
+      <c r="I9" s="25">
         <f>167.12*10^7</f>
         <v>1671200000</v>
       </c>
-      <c r="K9" s="25">
+      <c r="J9" s="25">
         <v>36500000</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>51</v>
       </c>
@@ -7058,15 +7449,15 @@
       <c r="H10" s="13">
         <v>0</v>
       </c>
-      <c r="J10" s="25">
+      <c r="I10" s="25">
         <f>24.27*10^7</f>
         <v>242700000</v>
       </c>
-      <c r="K10" s="25">
+      <c r="J10" s="25">
         <v>10500000</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>52</v>
       </c>
@@ -7091,15 +7482,15 @@
       <c r="H11" s="13">
         <v>0</v>
       </c>
-      <c r="J11" s="25">
+      <c r="I11" s="25">
         <f>31.18*10^7</f>
         <v>311800000</v>
       </c>
-      <c r="K11" s="25">
+      <c r="J11" s="25">
         <v>11900000</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>46</v>
       </c>
@@ -7124,15 +7515,15 @@
       <c r="H12" s="13">
         <v>0</v>
       </c>
-      <c r="J12" s="25">
+      <c r="I12" s="25">
         <f>104.68*10^7</f>
         <v>1046800000.0000001</v>
       </c>
-      <c r="K12" s="25">
+      <c r="J12" s="25">
         <v>22400000.000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>53</v>
       </c>
@@ -7157,15 +7548,15 @@
       <c r="H13" s="13">
         <v>0</v>
       </c>
-      <c r="J13" s="28">
+      <c r="I13" s="28">
         <f>269.89*10^7</f>
         <v>2698900000</v>
       </c>
-      <c r="K13" s="28">
+      <c r="J13" s="28">
         <v>47300000.000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>54</v>
       </c>
@@ -7190,15 +7581,15 @@
       <c r="H14" s="13">
         <v>0</v>
       </c>
-      <c r="J14" s="28">
+      <c r="I14" s="28">
         <f>246.53*10^7</f>
         <v>2465300000</v>
       </c>
-      <c r="K14" s="28">
+      <c r="J14" s="28">
         <v>42900000</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>55</v>
       </c>
@@ -7223,14 +7614,14 @@
       <c r="H15" s="13">
         <v>0</v>
       </c>
+      <c r="I15" s="28">
+        <v>1414100000</v>
+      </c>
       <c r="J15" s="28">
-        <v>1414100000</v>
-      </c>
-      <c r="K15" s="28">
         <v>25200000</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>56</v>
       </c>
@@ -7255,14 +7646,14 @@
       <c r="H16" s="13">
         <v>0</v>
       </c>
+      <c r="I16" s="28">
+        <v>1648000000</v>
+      </c>
       <c r="J16" s="28">
-        <v>1648000000</v>
-      </c>
-      <c r="K16" s="28">
         <v>28400000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>57</v>
       </c>
@@ -7287,14 +7678,14 @@
       <c r="H17" s="13">
         <v>0</v>
       </c>
+      <c r="I17" s="28">
+        <v>2350000000</v>
+      </c>
       <c r="J17" s="28">
-        <v>2350000000</v>
-      </c>
-      <c r="K17" s="28">
         <v>40400000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>58</v>
       </c>
@@ -7319,14 +7710,14 @@
       <c r="H18" s="13">
         <v>0</v>
       </c>
+      <c r="I18" s="28">
+        <v>901900000</v>
+      </c>
       <c r="J18" s="28">
-        <v>901900000</v>
-      </c>
-      <c r="K18" s="28">
         <v>19700000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>59</v>
       </c>
@@ -7351,14 +7742,14 @@
       <c r="H19" s="13">
         <v>0</v>
       </c>
+      <c r="I19" s="29">
+        <v>1078000000</v>
+      </c>
       <c r="J19" s="29">
-        <v>1078000000</v>
-      </c>
-      <c r="K19" s="29">
         <v>27700000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>60</v>
       </c>
@@ -7383,14 +7774,14 @@
       <c r="H20" s="13">
         <v>0</v>
       </c>
+      <c r="I20" s="25">
+        <v>1024900000</v>
+      </c>
       <c r="J20" s="25">
-        <v>1024900000</v>
-      </c>
-      <c r="K20" s="25">
         <v>24800000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>61</v>
       </c>
@@ -7415,14 +7806,14 @@
       <c r="H21" s="13">
         <v>0</v>
       </c>
-      <c r="J21" s="30">
+      <c r="I21" s="30">
         <v>2989600000</v>
       </c>
-      <c r="K21" s="25">
+      <c r="J21" s="25">
         <v>32000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>47</v>
       </c>
@@ -7447,14 +7838,14 @@
       <c r="H22" s="13">
         <v>0</v>
       </c>
+      <c r="I22" s="25">
+        <v>1942300000</v>
+      </c>
       <c r="J22" s="25">
-        <v>1942300000</v>
-      </c>
-      <c r="K22" s="25">
         <v>46700000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>48</v>
       </c>
@@ -7479,14 +7870,14 @@
       <c r="H23" s="13">
         <v>0</v>
       </c>
+      <c r="I23" s="25">
+        <v>3102600000</v>
+      </c>
       <c r="J23" s="25">
-        <v>3102600000</v>
-      </c>
-      <c r="K23" s="25">
         <v>82300000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>62</v>
       </c>
@@ -7511,14 +7902,14 @@
       <c r="H24" s="13">
         <v>0</v>
       </c>
+      <c r="I24" s="25">
+        <v>2691600000.0000005</v>
+      </c>
       <c r="J24" s="25">
-        <v>2691600000.0000005</v>
-      </c>
-      <c r="K24" s="25">
         <v>61800000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>63</v>
       </c>
@@ -7543,14 +7934,14 @@
       <c r="H25" s="13">
         <v>0</v>
       </c>
+      <c r="I25" s="28">
+        <v>2771500000</v>
+      </c>
       <c r="J25" s="28">
-        <v>2771500000</v>
-      </c>
-      <c r="K25" s="28">
         <v>52000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>64</v>
       </c>
@@ -7575,14 +7966,14 @@
       <c r="H26" s="13">
         <v>0</v>
       </c>
+      <c r="I26" s="28">
+        <v>654000000</v>
+      </c>
       <c r="J26" s="28">
-        <v>654000000</v>
-      </c>
-      <c r="K26" s="28">
         <v>15000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>65</v>
       </c>
@@ -7607,14 +7998,14 @@
       <c r="H27" s="13">
         <v>0</v>
       </c>
+      <c r="I27" s="32">
+        <v>412900000</v>
+      </c>
       <c r="J27" s="32">
-        <v>412900000</v>
-      </c>
-      <c r="K27" s="32">
         <v>7200000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>66</v>
       </c>
@@ -7639,14 +8030,14 @@
       <c r="H28" s="13">
         <v>0</v>
       </c>
+      <c r="I28" s="33">
+        <v>388000000</v>
+      </c>
       <c r="J28" s="33">
-        <v>388000000</v>
-      </c>
-      <c r="K28" s="33">
         <v>7700000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>67</v>
       </c>
@@ -7671,33 +8062,98 @@
       <c r="H29" s="13">
         <v>0</v>
       </c>
+      <c r="I29" s="32">
+        <v>425000000</v>
+      </c>
       <c r="J29" s="32">
-        <v>425000000</v>
-      </c>
-      <c r="K29" s="32">
         <v>9500000</v>
       </c>
     </row>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="12"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="Q49" s="1"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="Q50" s="1"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="Q51" s="1"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="12"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="Q52" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7708,7 +8164,7 @@
   <dimension ref="A1:BT16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD16"/>
+      <selection activeCell="A2" sqref="A2:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7716,54 +8172,57 @@
     <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:72" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="F1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="N1" t="s">
+      <c r="M1" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="N1" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
+      <c r="O1" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="P1" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Q1" s="66" t="s">
         <v>38</v>
+      </c>
+      <c r="R1" s="66" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:72" s="45" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -7791,28 +8250,31 @@
       <c r="H2" s="45">
         <v>0</v>
       </c>
-      <c r="J2" s="44">
+      <c r="I2" s="44">
         <f>3.87*10000000</f>
         <v>38700000</v>
       </c>
-      <c r="K2" s="44">
+      <c r="J2" s="44">
         <v>3700000</v>
       </c>
-      <c r="L2" s="41"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45">
+        <v>4</v>
+      </c>
       <c r="M2" s="45">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N2" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="45">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P2" s="45">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R2" s="45">
         <v>0</v>
@@ -7843,13 +8305,14 @@
       <c r="H3" s="45">
         <v>0</v>
       </c>
-      <c r="J3" s="44">
+      <c r="I3" s="44">
         <f>3.79*10000000</f>
         <v>37900000</v>
       </c>
-      <c r="K3" s="44">
+      <c r="J3" s="44">
         <v>2500000</v>
       </c>
+      <c r="K3" s="44"/>
       <c r="L3" s="41"/>
     </row>
     <row r="4" spans="1:72" s="45" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -7877,13 +8340,14 @@
       <c r="H4" s="45">
         <v>0</v>
       </c>
-      <c r="J4" s="44">
+      <c r="I4" s="44">
         <f>0.95*10000000</f>
         <v>9500000</v>
       </c>
-      <c r="K4" s="44">
+      <c r="J4" s="44">
         <v>1500000</v>
       </c>
+      <c r="K4" s="44"/>
       <c r="L4" s="41"/>
       <c r="N4" s="41"/>
     </row>
@@ -7912,13 +8376,14 @@
       <c r="H5" s="45">
         <v>0</v>
       </c>
-      <c r="J5" s="44">
+      <c r="I5" s="44">
         <f>0.42*10000000</f>
         <v>4200000</v>
       </c>
-      <c r="K5" s="44">
+      <c r="J5" s="44">
         <v>1300000</v>
       </c>
+      <c r="K5" s="44"/>
       <c r="L5" s="41"/>
     </row>
     <row r="6" spans="1:72" s="45" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -7946,13 +8411,14 @@
       <c r="H6" s="45">
         <v>0</v>
       </c>
-      <c r="J6" s="44">
+      <c r="I6" s="44">
         <f>1.11*10000000</f>
         <v>11100000.000000002</v>
       </c>
-      <c r="K6" s="44">
+      <c r="J6" s="44">
         <v>2000000</v>
       </c>
+      <c r="K6" s="44"/>
       <c r="L6" s="41"/>
     </row>
     <row r="7" spans="1:72" s="45" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -7980,12 +8446,13 @@
       <c r="H7" s="45">
         <v>0</v>
       </c>
+      <c r="I7" s="44">
+        <v>5800000</v>
+      </c>
       <c r="J7" s="44">
-        <v>5800000</v>
-      </c>
-      <c r="K7" s="44">
         <v>800000</v>
       </c>
+      <c r="K7" s="44"/>
       <c r="L7" s="41"/>
     </row>
     <row r="8" spans="1:72" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -8013,12 +8480,13 @@
       <c r="H8" s="45">
         <v>0</v>
       </c>
+      <c r="I8" s="44">
+        <v>6850000.0000000009</v>
+      </c>
       <c r="J8" s="44">
-        <v>6850000.0000000009</v>
-      </c>
-      <c r="K8" s="44">
         <v>800000</v>
       </c>
+      <c r="K8" s="44"/>
       <c r="L8" s="41"/>
     </row>
     <row r="9" spans="1:72" s="47" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -8046,12 +8514,13 @@
       <c r="H9" s="45">
         <v>0</v>
       </c>
+      <c r="I9" s="44">
+        <v>1400000.0000000002</v>
+      </c>
       <c r="J9" s="44">
-        <v>1400000.0000000002</v>
-      </c>
-      <c r="K9" s="44">
         <v>200000</v>
       </c>
+      <c r="K9" s="44"/>
       <c r="L9" s="41"/>
     </row>
     <row r="10" spans="1:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -8079,12 +8548,13 @@
       <c r="H10" s="45">
         <v>0</v>
       </c>
+      <c r="I10" s="39">
+        <v>75000000</v>
+      </c>
       <c r="J10" s="39">
-        <v>75000000</v>
-      </c>
-      <c r="K10" s="39">
         <v>4400000</v>
       </c>
+      <c r="K10" s="39"/>
       <c r="L10" s="41"/>
       <c r="M10" s="45"/>
       <c r="N10" s="45"/>
@@ -8172,12 +8642,13 @@
       <c r="H11" s="45">
         <v>0</v>
       </c>
+      <c r="I11" s="39">
+        <v>78700000</v>
+      </c>
       <c r="J11" s="39">
-        <v>78700000</v>
-      </c>
-      <c r="K11" s="39">
         <v>6400000</v>
       </c>
+      <c r="K11" s="39"/>
       <c r="L11" s="41"/>
       <c r="M11" s="45"/>
       <c r="N11" s="45"/>
@@ -8265,12 +8736,13 @@
       <c r="H12" s="45">
         <v>0</v>
       </c>
+      <c r="I12" s="38">
+        <v>167400000</v>
+      </c>
       <c r="J12" s="38">
-        <v>167400000</v>
-      </c>
-      <c r="K12" s="38">
         <v>9900000</v>
       </c>
+      <c r="K12" s="38"/>
       <c r="L12" s="41"/>
       <c r="M12" s="45"/>
       <c r="N12" s="45"/>
@@ -8358,12 +8830,13 @@
       <c r="H13" s="45">
         <v>0</v>
       </c>
+      <c r="I13" s="52">
+        <v>331000000</v>
+      </c>
       <c r="J13" s="52">
-        <v>331000000</v>
-      </c>
-      <c r="K13" s="52">
         <v>13400000</v>
       </c>
+      <c r="K13" s="52"/>
       <c r="L13" s="41"/>
     </row>
     <row r="14" spans="1:72" s="55" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -8391,12 +8864,13 @@
       <c r="H14" s="45">
         <v>0</v>
       </c>
+      <c r="I14" s="54">
+        <v>199100000</v>
+      </c>
       <c r="J14" s="54">
-        <v>199100000</v>
-      </c>
-      <c r="K14" s="54">
         <v>7600000</v>
       </c>
+      <c r="K14" s="54"/>
       <c r="L14" s="41"/>
     </row>
     <row r="15" spans="1:72" s="45" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -8424,12 +8898,13 @@
       <c r="H15" s="45">
         <v>0</v>
       </c>
+      <c r="I15" s="44">
+        <v>72400000</v>
+      </c>
       <c r="J15" s="44">
-        <v>72400000</v>
-      </c>
-      <c r="K15" s="44">
         <v>6200000</v>
       </c>
+      <c r="K15" s="44"/>
       <c r="L15" s="41"/>
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.2">
@@ -8444,7 +8919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24694F2A-853A-E44C-A507-6368D3EEDD55}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated exposure age script dependencies, removed unneccesary scripts
</commit_message>
<xml_diff>
--- a/src/Data/Inputs.xlsx
+++ b/src/Data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EE0161-2E70-BD47-B170-788C35B852E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC95080C-2114-C449-9E65-B7BB7209E71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="1" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="139">
   <si>
     <t>Sample Name</t>
   </si>
@@ -548,6 +548,9 @@
   </si>
   <si>
     <t xml:space="preserve"> in g/cm2/yr</t>
+  </si>
+  <si>
+    <t>If you do not provide a long enough duration to produce the amount of nuclide specified, you will receive a python generated error in line 92 (for 3He) OR line 202 (for 21Ne)</t>
   </si>
 </sst>
 </file>
@@ -733,7 +736,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -885,12 +888,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1059,9 +1082,6 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1095,6 +1115,21 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1105,12 +1140,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1125,20 +1154,26 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1455,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
-  <dimension ref="A1:S84"/>
+  <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1470,318 +1505,623 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="S1" s="66" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="10">
-        <v>38</v>
-      </c>
-      <c r="C2" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D2" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E2" s="1">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="34">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C2" s="34">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D2" s="34">
+        <v>957</v>
+      </c>
+      <c r="E2" s="35">
+        <v>3</v>
+      </c>
+      <c r="F2" s="34">
+        <v>2.65</v>
+      </c>
+      <c r="G2" s="35">
+        <v>1</v>
+      </c>
+      <c r="H2" s="35">
+        <v>0</v>
+      </c>
+      <c r="I2" s="34">
+        <v>458399999.99999994</v>
+      </c>
+      <c r="J2" s="38">
+        <v>2200000</v>
+      </c>
+      <c r="L2" s="37">
         <v>4</v>
       </c>
-      <c r="F2" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11">
-        <f>3*10^-3</f>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I2" s="2">
-        <v>2380000</v>
-      </c>
-      <c r="J2" s="2">
-        <v>56000</v>
-      </c>
-      <c r="L2">
-        <v>4</v>
-      </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2">
-        <v>27.5</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>28.201000000000001</v>
+        <v>20</v>
       </c>
       <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>15</v>
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="10">
-        <v>38</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D3" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="11">
-        <f>10*10^-3</f>
-        <v>0.01</v>
-      </c>
-      <c r="I3" s="2">
-        <v>2630000</v>
-      </c>
-      <c r="J3" s="7">
-        <v>59000</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="10">
-        <v>38</v>
-      </c>
-      <c r="C4" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D4" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="11">
-        <f>20*10^-3</f>
-        <v>0.02</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2750000</v>
-      </c>
-      <c r="J4" s="7">
-        <v>57000</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="10">
-        <v>38</v>
-      </c>
-      <c r="C5" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D5" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="2">
-        <v>330000</v>
-      </c>
-      <c r="J5" s="7">
-        <v>550000</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="10">
-        <v>38</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D6" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="2">
-        <v>730000</v>
-      </c>
-      <c r="J6" s="7">
-        <v>540000</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="10">
-        <v>38</v>
-      </c>
-      <c r="C7" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="2">
-        <v>340000</v>
-      </c>
-      <c r="J7" s="7">
-        <v>600000</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="10">
-        <v>38</v>
-      </c>
-      <c r="C8" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D8" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="2">
-        <v>590000</v>
-      </c>
-      <c r="J8" s="7">
-        <v>560000</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>55</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="34">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C3" s="34">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D3" s="34">
+        <v>957</v>
+      </c>
+      <c r="E3" s="35">
+        <v>3</v>
+      </c>
+      <c r="F3" s="34">
+        <v>2.65</v>
+      </c>
+      <c r="G3" s="35">
+        <v>1</v>
+      </c>
+      <c r="H3" s="35">
+        <v>0</v>
+      </c>
+      <c r="I3" s="34">
+        <v>458399999.99999994</v>
+      </c>
+      <c r="J3" s="38">
+        <v>2200000</v>
+      </c>
+      <c r="M3" s="37"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="35">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C4" s="35">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D4" s="35">
+        <v>957</v>
+      </c>
+      <c r="E4" s="35">
+        <v>3</v>
+      </c>
+      <c r="F4" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G4" s="35">
+        <v>1</v>
+      </c>
+      <c r="H4" s="35">
+        <v>0</v>
+      </c>
+      <c r="I4" s="35">
+        <v>495000000</v>
+      </c>
+      <c r="J4" s="39">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="35">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C5" s="35">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D5" s="35">
+        <v>957</v>
+      </c>
+      <c r="E5" s="35">
+        <v>3</v>
+      </c>
+      <c r="F5" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G5" s="35">
+        <v>1</v>
+      </c>
+      <c r="H5" s="35">
+        <v>0</v>
+      </c>
+      <c r="I5" s="35">
+        <v>381800000</v>
+      </c>
+      <c r="J5" s="39">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="35">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C6" s="35">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D6" s="35">
+        <v>957</v>
+      </c>
+      <c r="E6" s="35">
+        <v>3</v>
+      </c>
+      <c r="F6" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="35">
+        <v>0</v>
+      </c>
+      <c r="I6" s="35">
+        <v>725300000</v>
+      </c>
+      <c r="J6" s="39">
+        <v>4400000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="35">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C7" s="35">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D7" s="35">
+        <v>957</v>
+      </c>
+      <c r="E7" s="35">
+        <v>3</v>
+      </c>
+      <c r="F7" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G7" s="35">
+        <v>1</v>
+      </c>
+      <c r="H7" s="35">
+        <v>0</v>
+      </c>
+      <c r="I7" s="35">
+        <v>463100000</v>
+      </c>
+      <c r="J7" s="39">
+        <v>3300000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="35">
+        <v>-19.564599999999999</v>
+      </c>
+      <c r="C8" s="35">
+        <v>-70.117283</v>
+      </c>
+      <c r="D8" s="35">
+        <v>925</v>
+      </c>
+      <c r="E8" s="35">
+        <v>3</v>
+      </c>
+      <c r="F8" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G8" s="35">
+        <v>1</v>
+      </c>
+      <c r="H8" s="35">
+        <v>0</v>
+      </c>
+      <c r="I8" s="35">
+        <v>501800000</v>
+      </c>
+      <c r="J8" s="39">
+        <v>3400000.0000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="35">
+        <v>-19.564599999999999</v>
+      </c>
+      <c r="C9" s="35">
+        <v>-70.117283</v>
+      </c>
+      <c r="D9" s="35">
+        <v>925</v>
+      </c>
+      <c r="E9" s="35">
+        <v>3</v>
+      </c>
+      <c r="F9" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G9" s="35">
+        <v>1</v>
+      </c>
+      <c r="H9" s="35">
+        <v>0</v>
+      </c>
+      <c r="I9" s="35">
+        <v>315000000</v>
+      </c>
+      <c r="J9" s="39">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="35">
+        <v>-19.564599999999999</v>
+      </c>
+      <c r="C10" s="35">
+        <v>-70.117283</v>
+      </c>
+      <c r="D10" s="35">
+        <v>925</v>
+      </c>
+      <c r="E10" s="35">
+        <v>3</v>
+      </c>
+      <c r="F10" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G10" s="35">
+        <v>1</v>
+      </c>
+      <c r="H10" s="35">
+        <v>0</v>
+      </c>
+      <c r="I10" s="35">
+        <v>209900000.00000003</v>
+      </c>
+      <c r="J10" s="39">
+        <v>1600000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="35">
+        <v>-19.564599999999999</v>
+      </c>
+      <c r="C11" s="35">
+        <v>-70.117283</v>
+      </c>
+      <c r="D11" s="35">
+        <v>925</v>
+      </c>
+      <c r="E11" s="35">
+        <v>3</v>
+      </c>
+      <c r="F11" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G11" s="35">
+        <v>1</v>
+      </c>
+      <c r="H11" s="35">
+        <v>0</v>
+      </c>
+      <c r="I11" s="35">
+        <v>498800000</v>
+      </c>
+      <c r="J11" s="39">
+        <v>3100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="35">
+        <v>-19.565581999999999</v>
+      </c>
+      <c r="C12" s="35">
+        <v>-70.110219999999998</v>
+      </c>
+      <c r="D12" s="35">
+        <v>931</v>
+      </c>
+      <c r="E12" s="35">
+        <v>3</v>
+      </c>
+      <c r="F12" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G12" s="35">
+        <v>1</v>
+      </c>
+      <c r="H12" s="35">
+        <v>0</v>
+      </c>
+      <c r="I12" s="35">
+        <v>313400000</v>
+      </c>
+      <c r="J12" s="39">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="35">
+        <v>-19.565581999999999</v>
+      </c>
+      <c r="C13" s="35">
+        <v>-70.110219999999998</v>
+      </c>
+      <c r="D13" s="35">
+        <v>931</v>
+      </c>
+      <c r="E13" s="35">
+        <v>3</v>
+      </c>
+      <c r="F13" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G13" s="35">
+        <v>1</v>
+      </c>
+      <c r="H13" s="35">
+        <v>0</v>
+      </c>
+      <c r="I13" s="35">
+        <v>415200000.00000006</v>
+      </c>
+      <c r="J13" s="39">
+        <v>2800000.0000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="35">
+        <v>-19.565581999999999</v>
+      </c>
+      <c r="C14" s="35">
+        <v>-70.110219999999998</v>
+      </c>
+      <c r="D14" s="35">
+        <v>931</v>
+      </c>
+      <c r="E14" s="35">
+        <v>3</v>
+      </c>
+      <c r="F14" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G14" s="35">
+        <v>1</v>
+      </c>
+      <c r="H14" s="35">
+        <v>0</v>
+      </c>
+      <c r="I14" s="35">
+        <v>534600000</v>
+      </c>
+      <c r="J14" s="39">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="35">
+        <v>-19.565581999999999</v>
+      </c>
+      <c r="C15" s="35">
+        <v>-70.110219999999998</v>
+      </c>
+      <c r="D15" s="35">
+        <v>931</v>
+      </c>
+      <c r="E15" s="35">
+        <v>3</v>
+      </c>
+      <c r="F15" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G15" s="35">
+        <v>1</v>
+      </c>
+      <c r="H15" s="35">
+        <v>0</v>
+      </c>
+      <c r="I15" s="35">
+        <v>396300000</v>
+      </c>
+      <c r="J15" s="39">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="35">
+        <v>-19.551714</v>
+      </c>
+      <c r="C16" s="35">
+        <v>-70.076702999999995</v>
+      </c>
+      <c r="D16" s="35">
+        <v>1023</v>
+      </c>
+      <c r="E16" s="35">
+        <v>3</v>
+      </c>
+      <c r="F16" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G16" s="35">
+        <v>1</v>
+      </c>
+      <c r="H16" s="35">
+        <v>0</v>
+      </c>
+      <c r="I16" s="35">
+        <v>1799999.9999999998</v>
+      </c>
+      <c r="J16" s="39">
+        <v>700000.00000000012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="35">
+        <v>-19.551714</v>
+      </c>
+      <c r="C17" s="35">
+        <v>-70.076702999999995</v>
+      </c>
+      <c r="D17" s="35">
+        <v>1023</v>
+      </c>
+      <c r="E17" s="35">
+        <v>3</v>
+      </c>
+      <c r="F17" s="35">
+        <v>2.65</v>
+      </c>
+      <c r="G17" s="35">
+        <v>1</v>
+      </c>
+      <c r="H17" s="35">
+        <v>0</v>
+      </c>
+      <c r="I17" s="35">
+        <v>3400000.0000000005</v>
+      </c>
+      <c r="J17" s="39">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="36">
+        <v>-19.551714</v>
+      </c>
+      <c r="C18" s="36">
+        <v>-70.076702999999995</v>
+      </c>
+      <c r="D18" s="36">
+        <v>1023</v>
+      </c>
+      <c r="E18" s="35">
+        <v>3</v>
+      </c>
+      <c r="F18" s="36">
+        <v>2.65</v>
+      </c>
+      <c r="G18" s="35">
+        <v>1</v>
+      </c>
+      <c r="H18" s="35">
+        <v>0</v>
+      </c>
+      <c r="I18" s="36">
+        <v>2300000</v>
+      </c>
+      <c r="J18" s="40">
+        <v>400000</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1954,56 +2294,56 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3041,56 +3381,56 @@
     <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:72" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3816,56 +4156,56 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4630,56 +4970,56 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6078,7 +6418,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD18"/>
+      <selection activeCell="A2" sqref="A2:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6670,10 +7010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6699,56 +7039,56 @@
     <col min="19" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6830,7 +7170,7 @@
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="H6" s="63"/>
+      <c r="H6" s="62"/>
       <c r="J6" s="59"/>
       <c r="K6" s="59"/>
     </row>
@@ -6838,7 +7178,7 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="H7" s="63"/>
+      <c r="H7" s="62"/>
       <c r="J7" s="59"/>
       <c r="K7" s="59"/>
     </row>
@@ -6846,7 +7186,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="H8" s="63"/>
+      <c r="H8" s="62"/>
       <c r="J8" s="59"/>
       <c r="K8" s="59"/>
     </row>
@@ -6854,7 +7194,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="H9" s="63"/>
+      <c r="H9" s="62"/>
       <c r="J9" s="59"/>
       <c r="K9" s="59"/>
     </row>
@@ -6862,7 +7202,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="H10" s="63"/>
+      <c r="H10" s="62"/>
       <c r="I10" s="59"/>
       <c r="J10" s="59"/>
     </row>
@@ -6870,212 +7210,220 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="H11" s="63"/>
+      <c r="H11" s="62"/>
       <c r="I11" s="59"/>
       <c r="J11" s="59"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="H12" s="63"/>
+      <c r="H12" s="62"/>
       <c r="I12" s="59"/>
       <c r="J12" s="59"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="H13" s="63"/>
+      <c r="H13" s="62"/>
       <c r="I13" s="59"/>
       <c r="J13" s="59"/>
-      <c r="L13" s="64"/>
+      <c r="L13" s="63"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-      <c r="H14" s="63"/>
+      <c r="H14" s="62"/>
       <c r="I14" s="59"/>
       <c r="J14" s="59"/>
     </row>
     <row r="15" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="79" t="s">
+      <c r="D15" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="79" t="s">
+      <c r="E15" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="80" t="s">
+      <c r="F15" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="G15" s="67" t="s">
+      <c r="G15" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="83" t="s">
+      <c r="H15" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="I15" s="84" t="s">
+      <c r="I15" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="J15" s="84" t="s">
+      <c r="J15" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="L15" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="M15" s="70" t="s">
+      <c r="M15" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="N15" s="67" t="s">
+      <c r="N15" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="O15" s="70" t="s">
+      <c r="O15" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="P15" s="67" t="s">
+      <c r="P15" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="Q15" s="73" t="s">
+      <c r="Q15" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="R15" s="62" t="s">
+      <c r="R15" s="72" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="79"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="81" t="s">
+      <c r="A16" s="76"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="83"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="L16" s="68" t="s">
+      <c r="H16" s="85"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
+      <c r="L16" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="M16" s="71" t="s">
+      <c r="M16" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="N16" s="68"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="68" t="s">
+      <c r="N16" s="67"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="R16" s="78" t="s">
+      <c r="R16" s="76" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="79"/>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="84"/>
-      <c r="L17" s="68" t="s">
+      <c r="A17" s="76"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
+      <c r="L17" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="N17" s="74" t="s">
+      <c r="N17" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="O17" s="76" t="s">
+      <c r="O17" s="80" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="68" t="s">
+      <c r="P17" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="R17" s="78"/>
+      <c r="R17" s="76"/>
     </row>
     <row r="18" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="79"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="81"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="L18" s="69" t="s">
+      <c r="A18" s="76"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77"/>
+      <c r="L18" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="N18" s="74"/>
-      <c r="O18" s="76"/>
-      <c r="P18" s="68" t="s">
+      <c r="N18" s="78"/>
+      <c r="O18" s="80"/>
+      <c r="P18" s="67" t="s">
         <v>123</v>
       </c>
-      <c r="R18" s="78"/>
+      <c r="R18" s="76"/>
     </row>
     <row r="19" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="G19" s="82"/>
+      <c r="G19" s="84"/>
       <c r="H19" s="86"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="77"/>
-      <c r="P19" s="68" t="s">
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="N19" s="79"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="R19" s="78"/>
+      <c r="R19" s="76"/>
     </row>
     <row r="20" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="H20" s="88"/>
-      <c r="P20" s="68" t="s">
+      <c r="H20" s="74"/>
+      <c r="O20" s="89" t="s">
+        <v>138</v>
+      </c>
+      <c r="P20" s="87" t="s">
         <v>125</v>
       </c>
-      <c r="R20" s="78"/>
+      <c r="R20" s="76"/>
     </row>
     <row r="21" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="H21" s="87"/>
-      <c r="P21" s="68" t="s">
+      <c r="H21" s="73"/>
+      <c r="O21" s="90"/>
+      <c r="P21" s="87" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="H22" s="87"/>
-      <c r="P22" s="69" t="s">
+      <c r="H22" s="73"/>
+      <c r="O22" s="90"/>
+      <c r="P22" s="88" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H23" s="87"/>
+      <c r="H23" s="73"/>
+      <c r="O23" s="90"/>
     </row>
     <row r="24" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H24" s="87"/>
+      <c r="H24" s="73"/>
+      <c r="O24" s="90"/>
     </row>
     <row r="25" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H25" s="87"/>
+      <c r="H25" s="73"/>
+      <c r="O25" s="90"/>
     </row>
     <row r="26" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H26" s="87"/>
+      <c r="H26" s="73"/>
+      <c r="O26" s="90"/>
     </row>
     <row r="27" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H27" s="87"/>
+      <c r="H27" s="73"/>
+      <c r="O27" s="90"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O28" s="91"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="J15:J19"/>
+  <mergeCells count="14">
     <mergeCell ref="N17:N19"/>
     <mergeCell ref="O17:O19"/>
     <mergeCell ref="R16:R20"/>
@@ -7084,6 +7432,12 @@
     <mergeCell ref="G16:G19"/>
     <mergeCell ref="H15:H19"/>
     <mergeCell ref="I15:I19"/>
+    <mergeCell ref="O20:O28"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="J15:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7106,59 +7460,59 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:19" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="S1" s="66" t="s">
+      <c r="S1" s="65" t="s">
         <v>135</v>
       </c>
     </row>
@@ -7775,59 +8129,59 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:19" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="S1" s="66" t="s">
+      <c r="S1" s="65" t="s">
         <v>135</v>
       </c>
     </row>
@@ -8437,56 +8791,56 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
@@ -8806,56 +9160,56 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
@@ -9905,56 +10259,56 @@
     <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
@@ -10069,56 +10423,56 @@
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="66" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
+    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="N1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="O1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="R1" s="65" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated muons script per Balco (2017) and Balco et al. (2019)
</commit_message>
<xml_diff>
--- a/src/Data/Inputs.xlsx
+++ b/src/Data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7066CB-23D6-F442-8DCA-C1146B1CCAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BC85D0-5D99-A245-B4D2-67A0F2245CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10440" yWindow="460" windowWidth="18360" windowHeight="16520" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="143">
   <si>
     <t>Sample Name</t>
   </si>
@@ -551,6 +551,18 @@
   </si>
   <si>
     <t>If you do not provide a long enough duration to produce the amount of nuclide specified, you will receive a python generated error in line 92 (for 3He) OR line 202 (for 21Ne)</t>
+  </si>
+  <si>
+    <t>Uplift/Subsidence</t>
+  </si>
+  <si>
+    <t>Positive for uplift</t>
+  </si>
+  <si>
+    <t>Negative for subsidence</t>
+  </si>
+  <si>
+    <t>in cm/yr</t>
   </si>
 </sst>
 </file>
@@ -913,7 +925,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1130,6 +1142,15 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1140,9 +1161,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1160,9 +1178,6 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1172,7 +1187,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1490,22 +1505,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
@@ -1531,284 +1547,576 @@
         <v>13</v>
       </c>
       <c r="I1" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="65" t="s">
+      <c r="K1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="M1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="65" t="s">
+      <c r="N1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="65" t="s">
+      <c r="O1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="65" t="s">
+      <c r="P1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="65" t="s">
+      <c r="Q1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="65" t="s">
+      <c r="R1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="S1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="10">
-        <v>-25</v>
-      </c>
-      <c r="C2" s="10">
-        <v>133</v>
-      </c>
-      <c r="D2" s="10">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>2000000</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="15">
+        <v>-20.101167</v>
+      </c>
+      <c r="C2" s="15">
+        <v>-69.491221999999993</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0</v>
+      </c>
+      <c r="E2" s="15">
+        <v>5</v>
+      </c>
+      <c r="F2" s="26">
+        <v>3.2</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13">
+        <v>0</v>
+      </c>
+      <c r="J2" s="27">
+        <f>3.23*10^7</f>
+        <v>32300000</v>
+      </c>
+      <c r="K2" s="27">
+        <v>4900000</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
         <v>2</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>65.2</v>
-      </c>
-      <c r="O2">
-        <v>66.5</v>
-      </c>
-      <c r="P2">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0</v>
-      </c>
       <c r="R2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="11"/>
+        <v>31.25</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="15">
+        <v>-20.101167</v>
+      </c>
+      <c r="C3" s="15">
+        <v>-69.491221999999993</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="15">
+        <v>5</v>
+      </c>
+      <c r="F3" s="26">
+        <v>3.2</v>
+      </c>
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0</v>
+      </c>
+      <c r="J3" s="27">
+        <f>3.23*10^7</f>
+        <v>32300000</v>
+      </c>
+      <c r="K3" s="27">
+        <v>4900000</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>100</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="7"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="25"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="19"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J38" s="1"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="Q48" s="1"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R48" s="1"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="Q49" s="1"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R49" s="1"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="Q50" s="1"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R50" s="1"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="Q51" s="1"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R51" s="1"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="12"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1821,7 +2129,7 @@
   <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD32"/>
+      <selection activeCell="A2" sqref="A2:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6561,10 +6869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6577,20 +6885,21 @@
     <col min="6" max="6" width="18.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39.5" style="5" customWidth="1"/>
     <col min="8" max="8" width="21.83203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="27.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="5"/>
+    <col min="9" max="9" width="30.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="27.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.6640625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="18.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5" style="5" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="65" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
@@ -6616,34 +6925,37 @@
         <v>13</v>
       </c>
       <c r="I1" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="65" t="s">
+      <c r="K1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="M1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="65" t="s">
+      <c r="N1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="65" t="s">
+      <c r="O1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="65" t="s">
+      <c r="P1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="65" t="s">
+      <c r="Q1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="65" t="s">
+      <c r="R1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="S1" s="65" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>98</v>
       </c>
@@ -6668,327 +6980,360 @@
       <c r="H2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="56" t="s">
-        <v>105</v>
+      <c r="I2" s="60" t="s">
+        <v>140</v>
       </c>
       <c r="J2" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="56" t="s">
+      <c r="K2" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="58"/>
+      <c r="M2" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="M2" s="61" t="s">
+      <c r="N2" s="61" t="s">
         <v>116</v>
-      </c>
-      <c r="N2" s="56" t="s">
-        <v>104</v>
       </c>
       <c r="O2" s="56" t="s">
         <v>104</v>
       </c>
       <c r="P2" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q2" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="Q2" s="56" t="s">
+      <c r="R2" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="R2" s="56" t="s">
+      <c r="S2" s="56" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="57"/>
       <c r="C3" s="57"/>
       <c r="H3" s="60"/>
-      <c r="J3" s="58"/>
+      <c r="I3" s="60" t="s">
+        <v>141</v>
+      </c>
       <c r="K3" s="58"/>
-    </row>
-    <row r="4" spans="1:18" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="L3" s="58"/>
+    </row>
+    <row r="4" spans="1:19" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="57"/>
       <c r="C4" s="57"/>
       <c r="H4" s="60"/>
-      <c r="J4" s="58"/>
+      <c r="I4" s="60"/>
       <c r="K4" s="58"/>
-    </row>
-    <row r="5" spans="1:18" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="L4" s="58"/>
+    </row>
+    <row r="5" spans="1:19" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="57"/>
       <c r="C5" s="57"/>
       <c r="H5" s="60"/>
-      <c r="J5" s="58"/>
+      <c r="I5" s="60"/>
       <c r="K5" s="58"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L5" s="58"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="H6" s="62"/>
-      <c r="J6" s="59"/>
+      <c r="I6" s="62"/>
       <c r="K6" s="59"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L6" s="59"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="H7" s="62"/>
-      <c r="J7" s="59"/>
+      <c r="I7" s="62"/>
       <c r="K7" s="59"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L7" s="59"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="H8" s="62"/>
-      <c r="J8" s="59"/>
+      <c r="I8" s="62"/>
       <c r="K8" s="59"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L8" s="59"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="H9" s="62"/>
-      <c r="J9" s="59"/>
+      <c r="I9" s="62"/>
       <c r="K9" s="59"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L9" s="59"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="H10" s="62"/>
-      <c r="I10" s="59"/>
+      <c r="I10" s="62"/>
       <c r="J10" s="59"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K10" s="59"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="H11" s="62"/>
-      <c r="I11" s="59"/>
+      <c r="I11" s="62"/>
       <c r="J11" s="59"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K11" s="59"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="H12" s="62"/>
-      <c r="I12" s="59"/>
+      <c r="I12" s="62"/>
       <c r="J12" s="59"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K12" s="59"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="H13" s="62"/>
-      <c r="I13" s="59"/>
+      <c r="I13" s="62"/>
       <c r="J13" s="59"/>
-      <c r="L13" s="63"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K13" s="59"/>
+      <c r="M13" s="63"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="59"/>
+      <c r="I14" s="62"/>
       <c r="J14" s="59"/>
-    </row>
-    <row r="15" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82" t="s">
+      <c r="K14" s="59"/>
+    </row>
+    <row r="15" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="92" t="s">
+      <c r="C15" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="D15" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="82" t="s">
+      <c r="E15" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="83" t="s">
+      <c r="F15" s="85" t="s">
         <v>106</v>
       </c>
       <c r="G15" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="86" t="s">
+      <c r="H15" s="88" t="s">
         <v>137</v>
       </c>
-      <c r="I15" s="88" t="s">
+      <c r="I15" s="89" t="s">
+        <v>142</v>
+      </c>
+      <c r="J15" s="80" t="s">
         <v>110</v>
       </c>
-      <c r="J15" s="88" t="s">
+      <c r="K15" s="80" t="s">
         <v>110</v>
       </c>
-      <c r="L15" s="66" t="s">
+      <c r="M15" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="M15" s="69" t="s">
+      <c r="N15" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="N15" s="66" t="s">
+      <c r="O15" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="O15" s="69" t="s">
+      <c r="P15" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="P15" s="66" t="s">
+      <c r="Q15" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="Q15" s="77" t="s">
+      <c r="R15" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="R15" s="72" t="s">
+      <c r="S15" s="72" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="82"/>
-      <c r="B16" s="92"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="84" t="s">
+    <row r="16" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="79"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="86"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="L16" s="67" t="s">
+      <c r="H16" s="88"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="M16" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="M16" s="70" t="s">
+      <c r="N16" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="N16" s="67"/>
-      <c r="O16" s="71"/>
-      <c r="P16" s="67" t="s">
+      <c r="O16" s="67"/>
+      <c r="P16" s="71"/>
+      <c r="Q16" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="R16" s="82" t="s">
+      <c r="S16" s="79" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="82"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="L17" s="67" t="s">
+    <row r="17" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="79"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="80"/>
+      <c r="M17" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="N17" s="78" t="s">
+      <c r="O17" s="81" t="s">
         <v>119</v>
       </c>
-      <c r="O17" s="80" t="s">
+      <c r="P17" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="P17" s="67" t="s">
+      <c r="Q17" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="R17" s="82"/>
-    </row>
-    <row r="18" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="82"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="88"/>
-      <c r="L18" s="68" t="s">
+      <c r="S17" s="79"/>
+    </row>
+    <row r="18" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="79"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="80"/>
+      <c r="M18" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="N18" s="78"/>
-      <c r="O18" s="80"/>
-      <c r="P18" s="67" t="s">
+      <c r="O18" s="81"/>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="67" t="s">
         <v>123</v>
       </c>
-      <c r="R18" s="82"/>
-    </row>
-    <row r="19" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="G19" s="85"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="88"/>
-      <c r="J19" s="88"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="67" t="s">
+      <c r="S18" s="79"/>
+    </row>
+    <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="G19" s="87"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="O19" s="82"/>
+      <c r="P19" s="84"/>
+      <c r="Q19" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="R19" s="82"/>
-    </row>
-    <row r="20" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="S19" s="79"/>
+    </row>
+    <row r="20" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="H20" s="74"/>
-      <c r="O20" s="89" t="s">
+      <c r="I20" s="73"/>
+      <c r="P20" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="P20" s="75" t="s">
+      <c r="Q20" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="R20" s="82"/>
-    </row>
-    <row r="21" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="S20" s="79"/>
+    </row>
+    <row r="21" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="H21" s="73"/>
-      <c r="O21" s="90"/>
-      <c r="P21" s="75" t="s">
+      <c r="I21" s="73"/>
+      <c r="P21" s="91"/>
+      <c r="Q21" s="75" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="H22" s="73"/>
-      <c r="O22" s="90"/>
-      <c r="P22" s="76" t="s">
+      <c r="I22" s="73"/>
+      <c r="P22" s="91"/>
+      <c r="Q22" s="76" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H23" s="73"/>
-      <c r="O23" s="90"/>
-    </row>
-    <row r="24" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="73"/>
+      <c r="P23" s="91"/>
+    </row>
+    <row r="24" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H24" s="73"/>
-      <c r="O24" s="90"/>
-    </row>
-    <row r="25" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="73"/>
+      <c r="P24" s="91"/>
+    </row>
+    <row r="25" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H25" s="73"/>
-      <c r="O25" s="90"/>
-    </row>
-    <row r="26" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I25" s="73"/>
+      <c r="P25" s="91"/>
+    </row>
+    <row r="26" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H26" s="73"/>
-      <c r="O26" s="90"/>
-    </row>
-    <row r="27" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I26" s="73"/>
+      <c r="P26" s="91"/>
+    </row>
+    <row r="27" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H27" s="73"/>
-      <c r="O27" s="90"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="O28" s="91"/>
+      <c r="I27" s="73"/>
+      <c r="P27" s="91"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P28" s="92"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="O17:O19"/>
+    <mergeCell ref="P17:P19"/>
+    <mergeCell ref="S16:S20"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="J15:J19"/>
+    <mergeCell ref="P20:P28"/>
+    <mergeCell ref="I15:I19"/>
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="D15:D18"/>
-    <mergeCell ref="J15:J19"/>
-    <mergeCell ref="N17:N19"/>
-    <mergeCell ref="O17:O19"/>
-    <mergeCell ref="R16:R20"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="I15:I19"/>
-    <mergeCell ref="O20:O28"/>
+    <mergeCell ref="K15:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated atmospheric depth calculation to be time varying with climate data
</commit_message>
<xml_diff>
--- a/src/Data/Inputs.xlsx
+++ b/src/Data/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BC85D0-5D99-A245-B4D2-67A0F2245CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C430526C-83A1-1D49-A477-2708346B0A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
@@ -1507,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1616,13 +1616,13 @@
         <v>4</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="Q2">
         <v>2</v>
@@ -1639,10 +1639,10 @@
         <v>39</v>
       </c>
       <c r="B3" s="15">
-        <v>-20.101167</v>
+        <v>0</v>
       </c>
       <c r="C3" s="15">
-        <v>-69.491221999999993</v>
+        <v>0</v>
       </c>
       <c r="D3" s="15">
         <v>1000</v>
@@ -1673,13 +1673,13 @@
         <v>4</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="Q3">
         <v>2</v>

</xml_diff>

<commit_message>
uncommented uplift/subsidence, cleaned stdatm=2
</commit_message>
<xml_diff>
--- a/src/Data/Inputs.xlsx
+++ b/src/Data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C430526C-83A1-1D49-A477-2708346B0A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230BA2C0-9C97-FB42-A7AF-A8E18ACA0D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="34840" yWindow="1920" windowWidth="28800" windowHeight="16480" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
@@ -1508,12 +1508,13 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="27.6640625" bestFit="1" customWidth="1"/>
@@ -1603,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="27">
         <f>3.23*10^7</f>
@@ -1622,10 +1623,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>25</v>
+        <v>27.4</v>
       </c>
       <c r="Q2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R2">
         <v>31.25</v>
@@ -1660,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="27">
         <f>3.23*10^7</f>
@@ -1679,10 +1680,10 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>25</v>
+        <v>27.4</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3">
         <v>100</v>

</xml_diff>

<commit_message>
Fixed error in Natoms for 21Ne
</commit_message>
<xml_diff>
--- a/src/Data/Inputs.xlsx
+++ b/src/Data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0ADFB7-E399-A747-836C-A61E56F58B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F02161E-FE70-784C-A0F1-134848B9EEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Dunai" sheetId="15" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$78,Active!$B$83,Active!$B$85,Active!$B$86</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$77,Active!$B$82,Active!$B$84,Active!$B$85</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">atm_depth_comparison!$B$79,atm_depth_comparison!$B$84,atm_depth_comparison!$B$86,atm_depth_comparison!$B$87</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'CRFB texposure'!$B$79,'CRFB texposure'!$B$84,'CRFB texposure'!$B$86,'CRFB texposure'!$B$87</definedName>
     <definedName name="solver_adj" localSheetId="5" hidden="1">'Deccan Texposure'!$B$79,'Deccan Texposure'!$B$84,'Deccan Texposure'!$B$86,'Deccan Texposure'!$B$87</definedName>
@@ -41,17 +41,17 @@
     <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$89</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$88</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">atm_depth_comparison!$B$90</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">'CRFB texposure'!$B$90</definedName>
     <definedName name="solver_lhs1" localSheetId="5" hidden="1">'Deccan Texposure'!$B$90</definedName>
     <definedName name="solver_lhs1" localSheetId="8" hidden="1">'Figure 3'!$B$85</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$56</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$55</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">atm_depth_comparison!$F$57</definedName>
     <definedName name="solver_lhs2" localSheetId="4" hidden="1">'CRFB texposure'!$F$57</definedName>
     <definedName name="solver_lhs2" localSheetId="5" hidden="1">'Deccan Texposure'!$F$57</definedName>
     <definedName name="solver_lhs2" localSheetId="8" hidden="1">'Figure 3'!$F$52</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$57</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$56</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">atm_depth_comparison!$F$58</definedName>
     <definedName name="solver_lhs3" localSheetId="4" hidden="1">'CRFB texposure'!$F$58</definedName>
     <definedName name="solver_lhs3" localSheetId="5" hidden="1">'Deccan Texposure'!$F$58</definedName>
@@ -71,7 +71,7 @@
     <definedName name="solver_num" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="8" hidden="1">3</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$55</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$54</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">atm_depth_comparison!$F$56</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">'CRFB texposure'!$F$56</definedName>
     <definedName name="solver_opt" localSheetId="5" hidden="1">'Deccan Texposure'!$F$56</definedName>
@@ -945,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1162,6 +1162,19 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1172,9 +1185,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1192,9 +1202,6 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1205,9 +1212,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1525,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1599,1818 +1603,664 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10">
-        <v>38</v>
-      </c>
-      <c r="C2" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D2" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34">
+        <v>0</v>
+      </c>
+      <c r="C2" s="34">
+        <v>0</v>
+      </c>
+      <c r="D2" s="34">
+        <v>0</v>
+      </c>
+      <c r="E2" s="35">
+        <v>1</v>
+      </c>
+      <c r="F2" s="34">
+        <v>3</v>
+      </c>
+      <c r="G2" s="35">
+        <v>1</v>
+      </c>
+      <c r="H2" s="35">
+        <v>0</v>
+      </c>
+      <c r="I2" s="35">
+        <v>0</v>
+      </c>
+      <c r="J2" s="34">
+        <v>0</v>
+      </c>
+      <c r="K2" s="38">
+        <v>0</v>
+      </c>
+      <c r="M2" s="37">
         <v>4</v>
       </c>
-      <c r="F2" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2">
-        <v>4</v>
-      </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2">
-        <v>27.5</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>28.201000000000001</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>10</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10">
-        <v>38</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D3" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="7"/>
-      <c r="R3" s="1">
-        <v>2</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
-        <v>2</v>
-      </c>
-      <c r="B4" s="10">
-        <v>38</v>
-      </c>
-      <c r="C4" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D4" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="11">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="7"/>
-      <c r="R4" s="1">
-        <v>4</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="39"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10">
-        <v>38</v>
-      </c>
-      <c r="C5" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D5" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="7"/>
-      <c r="R5" s="1">
-        <v>6</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10">
-        <v>38</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D6" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="7"/>
-      <c r="R6" s="1">
-        <v>8</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
-        <v>5</v>
-      </c>
-      <c r="B7" s="10">
-        <v>38</v>
-      </c>
-      <c r="C7" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="11">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="7"/>
-      <c r="R7" s="1">
-        <v>10</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="39"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="10">
-        <v>38</v>
-      </c>
-      <c r="C8" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D8" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="7"/>
-      <c r="R8" s="1">
-        <v>12</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="39"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="10">
-        <v>38</v>
-      </c>
-      <c r="C9" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D9" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E9" s="1">
-        <v>4</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="R9" s="1">
-        <v>14</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="39"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
-        <v>8</v>
-      </c>
-      <c r="B10" s="10">
-        <v>38</v>
-      </c>
-      <c r="C10" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E10" s="1">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="11">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="R10" s="1">
-        <v>16</v>
-      </c>
-      <c r="S10">
-        <v>1</v>
-      </c>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="39"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10">
-        <v>38</v>
-      </c>
-      <c r="C11" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D11" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E11" s="1">
-        <v>4</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="R11" s="1">
-        <v>18</v>
-      </c>
-      <c r="S11">
-        <v>1</v>
-      </c>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="39"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="10">
-        <v>38</v>
-      </c>
-      <c r="C12" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D12" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E12" s="1">
-        <v>4</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="11">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="R12" s="1">
-        <v>20</v>
-      </c>
-      <c r="S12">
-        <v>1</v>
-      </c>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="12">
-        <v>11</v>
-      </c>
-      <c r="B13" s="10">
-        <v>38</v>
-      </c>
-      <c r="C13" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D13" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E13" s="1">
-        <v>4</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="11">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="R13" s="1">
-        <v>22</v>
-      </c>
-      <c r="S13">
-        <v>1</v>
-      </c>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="39"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="10">
-        <v>38</v>
-      </c>
-      <c r="C14" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D14" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E14" s="1">
-        <v>4</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="11">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="R14" s="1">
-        <v>24</v>
-      </c>
-      <c r="S14">
-        <v>1</v>
-      </c>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="39"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="10">
-        <v>38</v>
-      </c>
-      <c r="C15" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D15" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E15" s="1">
-        <v>4</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="11">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="R15" s="1">
-        <v>26</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="39"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="12">
-        <v>14</v>
-      </c>
-      <c r="B16" s="10">
-        <v>38</v>
-      </c>
-      <c r="C16" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D16" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E16" s="1">
-        <v>4</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="11">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="R16" s="1">
-        <v>28</v>
-      </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="10">
-        <v>38</v>
-      </c>
-      <c r="C17" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D17" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E17" s="1">
-        <v>4</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="11">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="R17" s="1">
-        <v>30</v>
-      </c>
-      <c r="S17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" s="10">
-        <v>38</v>
-      </c>
-      <c r="C18" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D18" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E18" s="1">
-        <v>4</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="11">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="R18" s="1">
-        <v>32</v>
-      </c>
-      <c r="S18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="12">
-        <v>17</v>
-      </c>
-      <c r="B19" s="10">
-        <v>38</v>
-      </c>
-      <c r="C19" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D19" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E19" s="1">
-        <v>4</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="11">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
-      <c r="R19" s="1">
-        <v>34</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="10">
-        <v>38</v>
-      </c>
-      <c r="C20" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D20" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E20" s="1">
-        <v>4</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20" s="11">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0</v>
-      </c>
-      <c r="R20" s="1">
-        <v>36</v>
-      </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" s="10">
-        <v>38</v>
-      </c>
-      <c r="C21" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D21" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E21" s="1">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="11">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="R21" s="1">
-        <v>38</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A22" s="12">
-        <v>20</v>
-      </c>
-      <c r="B22" s="10">
-        <v>38</v>
-      </c>
-      <c r="C22" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D22" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E22" s="1">
-        <v>4</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="11">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0</v>
-      </c>
-      <c r="R22" s="1">
-        <v>40</v>
-      </c>
-      <c r="S22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="10">
-        <v>38</v>
-      </c>
-      <c r="C23" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D23" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E23" s="1">
-        <v>4</v>
-      </c>
-      <c r="F23" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" s="11">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
-      <c r="R23" s="1">
-        <v>42</v>
-      </c>
-      <c r="S23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" s="10">
-        <v>38</v>
-      </c>
-      <c r="C24" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D24" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E24" s="1">
-        <v>4</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G24" s="1">
-        <v>1</v>
-      </c>
-      <c r="H24" s="11">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
-      <c r="R24" s="1">
-        <v>44</v>
-      </c>
-      <c r="S24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="12">
-        <v>23</v>
-      </c>
-      <c r="B25" s="10">
-        <v>38</v>
-      </c>
-      <c r="C25" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D25" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E25" s="1">
-        <v>4</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="H25" s="11">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
-      <c r="R25" s="1">
-        <v>46</v>
-      </c>
-      <c r="S25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" s="10">
-        <v>38</v>
-      </c>
-      <c r="C26" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D26" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E26" s="1">
-        <v>4</v>
-      </c>
-      <c r="F26" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
-      <c r="H26" s="11">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
-      <c r="R26" s="1">
-        <v>48</v>
-      </c>
-      <c r="S26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" s="10">
-        <v>38</v>
-      </c>
-      <c r="C27" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D27" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E27" s="1">
-        <v>4</v>
-      </c>
-      <c r="F27" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1</v>
-      </c>
-      <c r="H27" s="11">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-      <c r="R27" s="1">
-        <v>50</v>
-      </c>
-      <c r="S27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="12">
-        <v>26</v>
-      </c>
-      <c r="B28" s="10">
-        <v>38</v>
-      </c>
-      <c r="C28" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D28" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E28" s="1">
-        <v>4</v>
-      </c>
-      <c r="F28" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G28" s="1">
-        <v>1</v>
-      </c>
-      <c r="H28" s="11">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-      <c r="R28" s="1">
-        <v>52</v>
-      </c>
-      <c r="S28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" s="10">
-        <v>38</v>
-      </c>
-      <c r="C29" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D29" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E29" s="1">
-        <v>4</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G29" s="1">
-        <v>1</v>
-      </c>
-      <c r="H29" s="11">
-        <v>0</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0</v>
-      </c>
-      <c r="R29" s="1">
-        <v>54</v>
-      </c>
-      <c r="S29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" s="10">
-        <v>38</v>
-      </c>
-      <c r="C30" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D30" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E30" s="1">
-        <v>4</v>
-      </c>
-      <c r="F30" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-      <c r="H30" s="11">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-      <c r="R30" s="1">
-        <v>56</v>
-      </c>
-      <c r="S30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="12">
-        <v>29</v>
-      </c>
-      <c r="B31" s="10">
-        <v>38</v>
-      </c>
-      <c r="C31" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D31" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E31" s="1">
-        <v>4</v>
-      </c>
-      <c r="F31" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G31" s="1">
-        <v>1</v>
-      </c>
-      <c r="H31" s="11">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1">
-        <v>0</v>
-      </c>
-      <c r="R31" s="1">
-        <v>58</v>
-      </c>
-      <c r="S31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32" s="10">
-        <v>38</v>
-      </c>
-      <c r="C32" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D32" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E32" s="1">
-        <v>4</v>
-      </c>
-      <c r="F32" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G32" s="1">
-        <v>1</v>
-      </c>
-      <c r="H32" s="11">
-        <v>0</v>
-      </c>
-      <c r="I32" s="1">
-        <v>0</v>
-      </c>
-      <c r="R32" s="1">
-        <v>60</v>
-      </c>
-      <c r="S32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" s="10">
-        <v>38</v>
-      </c>
-      <c r="C33" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D33" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E33" s="1">
-        <v>4</v>
-      </c>
-      <c r="F33" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G33" s="1">
-        <v>1</v>
-      </c>
-      <c r="H33" s="11">
-        <v>0</v>
-      </c>
-      <c r="I33" s="1">
-        <v>0</v>
-      </c>
-      <c r="R33" s="1">
-        <v>62</v>
-      </c>
-      <c r="S33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A34" s="12">
-        <v>32</v>
-      </c>
-      <c r="B34" s="10">
-        <v>38</v>
-      </c>
-      <c r="C34" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D34" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E34" s="1">
-        <v>4</v>
-      </c>
-      <c r="F34" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G34" s="1">
-        <v>1</v>
-      </c>
-      <c r="H34" s="11">
-        <v>0</v>
-      </c>
-      <c r="I34" s="1">
-        <v>0</v>
-      </c>
-      <c r="R34" s="1">
-        <v>64</v>
-      </c>
-      <c r="S34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" s="10">
-        <v>38</v>
-      </c>
-      <c r="C35" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D35" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E35" s="1">
-        <v>4</v>
-      </c>
-      <c r="F35" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G35" s="1">
-        <v>1</v>
-      </c>
-      <c r="H35" s="11">
-        <v>0</v>
-      </c>
-      <c r="I35" s="1">
-        <v>0</v>
-      </c>
-      <c r="R35" s="1">
-        <v>66</v>
-      </c>
-      <c r="S35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36" s="10">
-        <v>38</v>
-      </c>
-      <c r="C36" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D36" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E36" s="1">
-        <v>4</v>
-      </c>
-      <c r="F36" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G36" s="1">
-        <v>1</v>
-      </c>
-      <c r="H36" s="11">
-        <v>0</v>
-      </c>
-      <c r="I36" s="1">
-        <v>0</v>
-      </c>
-      <c r="R36" s="1">
-        <v>68</v>
-      </c>
-      <c r="S36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="12">
-        <v>35</v>
-      </c>
-      <c r="B37" s="10">
-        <v>38</v>
-      </c>
-      <c r="C37" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D37" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E37" s="1">
-        <v>4</v>
-      </c>
-      <c r="F37" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G37" s="1">
-        <v>1</v>
-      </c>
-      <c r="H37" s="11">
-        <v>0</v>
-      </c>
-      <c r="I37" s="1">
-        <v>0</v>
-      </c>
-      <c r="R37" s="1">
-        <v>70</v>
-      </c>
-      <c r="S37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38" s="10">
-        <v>38</v>
-      </c>
-      <c r="C38" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D38" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E38" s="1">
-        <v>4</v>
-      </c>
-      <c r="F38" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1</v>
-      </c>
-      <c r="H38" s="11">
-        <v>0</v>
-      </c>
-      <c r="I38" s="1">
-        <v>0</v>
-      </c>
-      <c r="R38" s="1">
-        <v>72</v>
-      </c>
-      <c r="S38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39" s="10">
-        <v>38</v>
-      </c>
-      <c r="C39" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D39" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E39" s="1">
-        <v>4</v>
-      </c>
-      <c r="F39" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G39" s="1">
-        <v>1</v>
-      </c>
-      <c r="H39" s="11">
-        <v>0</v>
-      </c>
-      <c r="I39" s="1">
-        <v>0</v>
-      </c>
-      <c r="R39" s="1">
-        <v>74</v>
-      </c>
-      <c r="S39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A40" s="12">
-        <v>38</v>
-      </c>
-      <c r="B40" s="10">
-        <v>38</v>
-      </c>
-      <c r="C40" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D40" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E40" s="1">
-        <v>4</v>
-      </c>
-      <c r="F40" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1</v>
-      </c>
-      <c r="H40" s="11">
-        <v>0</v>
-      </c>
-      <c r="I40" s="1">
-        <v>0</v>
-      </c>
-      <c r="R40" s="1">
-        <v>76</v>
-      </c>
-      <c r="S40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41" s="10">
-        <v>38</v>
-      </c>
-      <c r="C41" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D41" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E41" s="1">
-        <v>4</v>
-      </c>
-      <c r="F41" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G41" s="1">
-        <v>1</v>
-      </c>
-      <c r="H41" s="11">
-        <v>0</v>
-      </c>
-      <c r="I41" s="1">
-        <v>0</v>
-      </c>
-      <c r="R41" s="1">
-        <v>78</v>
-      </c>
-      <c r="S41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42" s="10">
-        <v>38</v>
-      </c>
-      <c r="C42" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D42" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E42" s="1">
-        <v>4</v>
-      </c>
-      <c r="F42" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G42" s="1">
-        <v>1</v>
-      </c>
-      <c r="H42" s="11">
-        <v>0</v>
-      </c>
-      <c r="I42" s="1">
-        <v>0</v>
-      </c>
-      <c r="R42" s="1">
-        <v>80</v>
-      </c>
-      <c r="S42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A43" s="12">
-        <v>41</v>
-      </c>
-      <c r="B43" s="10">
-        <v>38</v>
-      </c>
-      <c r="C43" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D43" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E43" s="1">
-        <v>4</v>
-      </c>
-      <c r="F43" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G43" s="1">
-        <v>1</v>
-      </c>
-      <c r="H43" s="11">
-        <v>0</v>
-      </c>
-      <c r="I43" s="1">
-        <v>0</v>
-      </c>
-      <c r="R43" s="1">
-        <v>82</v>
-      </c>
-      <c r="S43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>42</v>
-      </c>
-      <c r="B44" s="10">
-        <v>38</v>
-      </c>
-      <c r="C44" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D44" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E44" s="1">
-        <v>4</v>
-      </c>
-      <c r="F44" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-      <c r="H44" s="11">
-        <v>0</v>
-      </c>
-      <c r="I44" s="1">
-        <v>0</v>
-      </c>
-      <c r="R44" s="1">
-        <v>84</v>
-      </c>
-      <c r="S44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45" s="10">
-        <v>38</v>
-      </c>
-      <c r="C45" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D45" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E45" s="1">
-        <v>4</v>
-      </c>
-      <c r="F45" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G45" s="1">
-        <v>1</v>
-      </c>
-      <c r="H45" s="11">
-        <v>0</v>
-      </c>
-      <c r="I45" s="1">
-        <v>0</v>
-      </c>
-      <c r="R45" s="1">
-        <v>86</v>
-      </c>
-      <c r="S45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A46" s="12">
-        <v>44</v>
-      </c>
-      <c r="B46" s="10">
-        <v>38</v>
-      </c>
-      <c r="C46" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D46" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E46" s="1">
-        <v>4</v>
-      </c>
-      <c r="F46" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G46" s="1">
-        <v>1</v>
-      </c>
-      <c r="H46" s="11">
-        <v>0</v>
-      </c>
-      <c r="I46" s="1">
-        <v>0</v>
-      </c>
-      <c r="R46" s="1">
-        <v>88</v>
-      </c>
-      <c r="S46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>45</v>
-      </c>
-      <c r="B47" s="10">
-        <v>38</v>
-      </c>
-      <c r="C47" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D47" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E47" s="1">
-        <v>4</v>
-      </c>
-      <c r="F47" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G47" s="1">
-        <v>1</v>
-      </c>
-      <c r="H47" s="11">
-        <v>0</v>
-      </c>
-      <c r="I47" s="1">
-        <v>0</v>
-      </c>
-      <c r="R47" s="1">
-        <v>90</v>
-      </c>
-      <c r="S47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>46</v>
-      </c>
-      <c r="B48" s="10">
-        <v>38</v>
-      </c>
-      <c r="C48" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D48" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E48" s="1">
-        <v>4</v>
-      </c>
-      <c r="F48" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G48" s="1">
-        <v>1</v>
-      </c>
-      <c r="H48" s="11">
-        <v>0</v>
-      </c>
-      <c r="I48" s="1">
-        <v>0</v>
-      </c>
-      <c r="R48" s="1">
-        <v>92</v>
-      </c>
-      <c r="S48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A49" s="12">
-        <v>47</v>
-      </c>
-      <c r="B49" s="10">
-        <v>38</v>
-      </c>
-      <c r="C49" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D49" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E49" s="1">
-        <v>4</v>
-      </c>
-      <c r="F49" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G49" s="1">
-        <v>1</v>
-      </c>
-      <c r="H49" s="11">
-        <v>0</v>
-      </c>
-      <c r="I49" s="1">
-        <v>0</v>
-      </c>
-      <c r="R49" s="1">
-        <v>94</v>
-      </c>
-      <c r="S49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <v>48</v>
-      </c>
-      <c r="B50" s="10">
-        <v>38</v>
-      </c>
-      <c r="C50" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D50" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E50" s="1">
-        <v>4</v>
-      </c>
-      <c r="F50" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G50" s="1">
-        <v>1</v>
-      </c>
-      <c r="H50" s="11">
-        <v>0</v>
-      </c>
-      <c r="I50" s="1">
-        <v>0</v>
-      </c>
-      <c r="R50" s="1">
-        <v>96</v>
-      </c>
-      <c r="S50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>49</v>
-      </c>
-      <c r="B51" s="10">
-        <v>38</v>
-      </c>
-      <c r="C51" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D51" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E51" s="1">
-        <v>4</v>
-      </c>
-      <c r="F51" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G51" s="1">
-        <v>1</v>
-      </c>
-      <c r="H51" s="11">
-        <v>0</v>
-      </c>
-      <c r="I51" s="1">
-        <v>0</v>
-      </c>
-      <c r="R51" s="1">
-        <v>98</v>
-      </c>
-      <c r="S51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A52" s="12">
-        <v>50</v>
-      </c>
-      <c r="B52" s="10">
-        <v>38</v>
-      </c>
-      <c r="C52" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D52" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E52" s="1">
-        <v>4</v>
-      </c>
-      <c r="F52" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G52" s="1">
-        <v>1</v>
-      </c>
-      <c r="H52" s="11">
-        <v>0</v>
-      </c>
-      <c r="I52" s="1">
-        <v>0</v>
-      </c>
-      <c r="R52" s="1">
-        <v>100</v>
-      </c>
-      <c r="S52">
-        <v>1</v>
-      </c>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="39"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="40"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="1"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="1"/>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="1"/>
+      <c r="R26" s="1"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="12"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="1"/>
+      <c r="R27" s="1"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="1"/>
+      <c r="R28" s="1"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="1"/>
+      <c r="R29" s="1"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" s="12"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="1"/>
+      <c r="R30" s="1"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="1"/>
+      <c r="R31" s="1"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="1"/>
+      <c r="R32" s="1"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A33" s="12"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="1"/>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="1"/>
+      <c r="R34" s="1"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="1"/>
+      <c r="R35" s="1"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="1"/>
+      <c r="R36" s="1"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="1"/>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="1"/>
+      <c r="R38" s="1"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="1"/>
+      <c r="R39" s="1"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="1"/>
+      <c r="R40" s="1"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="1"/>
+      <c r="R41" s="1"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="1"/>
+      <c r="R42" s="1"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="1"/>
+      <c r="R43" s="1"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="1"/>
+      <c r="R44" s="1"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A45" s="12"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="1"/>
+      <c r="R45" s="1"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="1"/>
+      <c r="R46" s="1"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="1"/>
+      <c r="R47" s="1"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A48" s="12"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="1"/>
+      <c r="R48" s="1"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="1"/>
+      <c r="R49" s="1"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="1"/>
+      <c r="R50" s="1"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A51" s="12"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="1"/>
+      <c r="R51" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -5331,7 +4181,7 @@
   <dimension ref="A1:BT19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD15"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8376,7 +7226,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD17"/>
+      <selection sqref="A1:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8472,7 +7322,7 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="Q2">
         <v>2</v>
@@ -8970,7 +7820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D41264A-E03E-5D48-9DEA-948271C7B252}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -9915,7 +8765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
@@ -10161,37 +9011,37 @@
       <c r="K14" s="59"/>
     </row>
     <row r="15" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="93" t="s">
+      <c r="C15" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="D15" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="82" t="s">
+      <c r="E15" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="83" t="s">
+      <c r="F15" s="87" t="s">
         <v>106</v>
       </c>
       <c r="G15" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="86" t="s">
+      <c r="H15" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="I15" s="87" t="s">
+      <c r="I15" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="J15" s="88" t="s">
+      <c r="J15" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="88" t="s">
+      <c r="K15" s="82" t="s">
         <v>110</v>
       </c>
       <c r="M15" s="66" t="s">
@@ -10217,19 +9067,19 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="82"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="84" t="s">
+      <c r="A16" s="81"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="86"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="82"/>
       <c r="M16" s="67" t="s">
         <v>113</v>
       </c>
@@ -10241,86 +9091,86 @@
       <c r="Q16" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="S16" s="82" t="s">
+      <c r="S16" s="81" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="82"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="92"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
       <c r="M17" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="O17" s="78" t="s">
+      <c r="O17" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="P17" s="80" t="s">
+      <c r="P17" s="85" t="s">
         <v>121</v>
       </c>
       <c r="Q17" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="S17" s="82"/>
+      <c r="S17" s="81"/>
     </row>
     <row r="18" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="82"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="88"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82"/>
       <c r="M18" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="O18" s="78"/>
-      <c r="P18" s="80"/>
+      <c r="O18" s="83"/>
+      <c r="P18" s="85"/>
       <c r="Q18" s="67" t="s">
         <v>123</v>
       </c>
-      <c r="S18" s="82"/>
+      <c r="S18" s="81"/>
     </row>
     <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="G19" s="85"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="92"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="88"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="81"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="91"/>
+      <c r="I19" s="95"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="82"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="86"/>
       <c r="Q19" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="82"/>
+      <c r="S19" s="81"/>
     </row>
     <row r="20" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="H20" s="74"/>
       <c r="I20" s="73"/>
-      <c r="P20" s="89" t="s">
+      <c r="P20" s="92" t="s">
         <v>138</v>
       </c>
       <c r="Q20" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="S20" s="82"/>
+      <c r="S20" s="81"/>
     </row>
     <row r="21" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="H21" s="73"/>
       <c r="I21" s="73"/>
-      <c r="P21" s="90"/>
+      <c r="P21" s="93"/>
       <c r="Q21" s="75" t="s">
         <v>126</v>
       </c>
@@ -10328,7 +9178,7 @@
     <row r="22" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="H22" s="73"/>
       <c r="I22" s="73"/>
-      <c r="P22" s="90"/>
+      <c r="P22" s="93"/>
       <c r="Q22" s="76" t="s">
         <v>127</v>
       </c>
@@ -10336,38 +9186,33 @@
     <row r="23" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H23" s="73"/>
       <c r="I23" s="73"/>
-      <c r="P23" s="90"/>
+      <c r="P23" s="93"/>
     </row>
     <row r="24" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H24" s="73"/>
       <c r="I24" s="73"/>
-      <c r="P24" s="90"/>
+      <c r="P24" s="93"/>
     </row>
     <row r="25" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H25" s="73"/>
       <c r="I25" s="73"/>
-      <c r="P25" s="90"/>
+      <c r="P25" s="93"/>
     </row>
     <row r="26" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H26" s="73"/>
       <c r="I26" s="73"/>
-      <c r="P26" s="90"/>
+      <c r="P26" s="93"/>
     </row>
     <row r="27" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H27" s="73"/>
       <c r="I27" s="73"/>
-      <c r="P27" s="90"/>
+      <c r="P27" s="93"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P28" s="91"/>
+      <c r="P28" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="K15:K19"/>
     <mergeCell ref="O17:O19"/>
     <mergeCell ref="P17:P19"/>
     <mergeCell ref="S16:S20"/>
@@ -10378,6 +9223,11 @@
     <mergeCell ref="J15:J19"/>
     <mergeCell ref="P20:P28"/>
     <mergeCell ref="I15:I19"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="K15:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated muons code for neon/LSDn compatibility
</commit_message>
<xml_diff>
--- a/src/Data/Inputs.xlsx
+++ b/src/Data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CBED11-F306-5B4D-A013-35FCA4FB1DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2520897E-1A56-6B42-8A08-837AAF3EB63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="19840" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="217">
   <si>
     <t>Sample Name</t>
   </si>
@@ -674,88 +674,52 @@
     <t>09-HAW-22-ol</t>
   </si>
   <si>
-    <t>Day 01-05</t>
-  </si>
-  <si>
-    <t>Day 02-02</t>
-  </si>
-  <si>
-    <t>21/10</t>
-  </si>
-  <si>
-    <t>20/10</t>
-  </si>
-  <si>
-    <t>Day 02-11</t>
-  </si>
-  <si>
-    <t>Day 4-02</t>
-  </si>
-  <si>
-    <t>Day 04-03</t>
-  </si>
-  <si>
-    <t>Day 4-04</t>
-  </si>
-  <si>
-    <t>Day 04-10</t>
-  </si>
-  <si>
-    <t>Day 04-11</t>
-  </si>
-  <si>
-    <t>Day 4-12</t>
-  </si>
-  <si>
-    <t>10/21</t>
-  </si>
-  <si>
-    <t>08/21</t>
-  </si>
-  <si>
-    <t>23/21</t>
-  </si>
-  <si>
-    <t>24/21</t>
-  </si>
-  <si>
-    <t>02/21</t>
-  </si>
-  <si>
-    <t>10/10</t>
-  </si>
-  <si>
-    <t>Day 03-10</t>
-  </si>
-  <si>
-    <t>Day 3 -11</t>
-  </si>
-  <si>
-    <t>01/02</t>
-  </si>
-  <si>
-    <t>Day 05-01</t>
-  </si>
-  <si>
-    <t>Day 05-02</t>
-  </si>
-  <si>
-    <t>Day 5 -03</t>
-  </si>
-  <si>
-    <t>01/12</t>
-  </si>
-  <si>
-    <t>02/12</t>
-  </si>
-  <si>
-    <t>07/18</t>
-  </si>
-  <si>
-    <t>06/16</t>
-  </si>
-  <si>
-    <t>09/16</t>
+    <t>p103/1</t>
+  </si>
+  <si>
+    <t>P103/A</t>
+  </si>
+  <si>
+    <t>P103/B</t>
+  </si>
+  <si>
+    <t>P103/C</t>
+  </si>
+  <si>
+    <t>P103/D</t>
+  </si>
+  <si>
+    <t>PI-06A</t>
+  </si>
+  <si>
+    <t>PI-06B</t>
+  </si>
+  <si>
+    <t>PI-06C</t>
+  </si>
+  <si>
+    <t>PI-06D</t>
+  </si>
+  <si>
+    <t>PI-07A</t>
+  </si>
+  <si>
+    <t>PI-07B</t>
+  </si>
+  <si>
+    <t>PI-07C</t>
+  </si>
+  <si>
+    <t>PI-07D</t>
+  </si>
+  <si>
+    <t>PI-11</t>
+  </si>
+  <si>
+    <t>PI-12</t>
+  </si>
+  <si>
+    <t>PI-01</t>
   </si>
 </sst>
 </file>
@@ -875,7 +839,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -903,6 +867,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1083,7 +1053,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1228,21 +1198,23 @@
     <xf numFmtId="2" fontId="6" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1254,6 +1226,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1271,6 +1246,9 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1283,6 +1261,10 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1601,7 +1583,7 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1672,43 +1654,41 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="9">
-        <v>-20.101167</v>
-      </c>
-      <c r="C2" s="9">
-        <v>-69.491221999999993</v>
-      </c>
-      <c r="D2" s="9">
-        <v>1380</v>
-      </c>
-      <c r="E2" s="9">
-        <v>5</v>
-      </c>
-      <c r="F2" s="10">
-        <v>3.2</v>
-      </c>
-      <c r="G2" s="8">
-        <v>1</v>
-      </c>
-      <c r="H2" s="8">
-        <v>0</v>
-      </c>
-      <c r="I2" s="8">
-        <v>0</v>
-      </c>
-      <c r="J2" s="51">
-        <f>3.23*10^7</f>
-        <v>32300000</v>
-      </c>
-      <c r="K2" s="51">
-        <v>4900000</v>
-      </c>
-      <c r="L2" s="50"/>
-      <c r="M2">
-        <v>2</v>
+      <c r="B2" s="52">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C2" s="52">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D2" s="52">
+        <v>957</v>
+      </c>
+      <c r="E2" s="50">
+        <v>3</v>
+      </c>
+      <c r="F2" s="52">
+        <v>2.65</v>
+      </c>
+      <c r="G2" s="50">
+        <v>1</v>
+      </c>
+      <c r="H2" s="50">
+        <v>0</v>
+      </c>
+      <c r="I2" s="50">
+        <v>0</v>
+      </c>
+      <c r="J2" s="52">
+        <v>458399999.99999994</v>
+      </c>
+      <c r="K2" s="53">
+        <v>2200000</v>
+      </c>
+      <c r="M2" s="72">
+        <v>4</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1717,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q2">
         <v>2</v>
@@ -1730,1042 +1710,730 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="B3" s="34">
-        <v>-20.101167</v>
-      </c>
-      <c r="C3" s="34">
-        <v>-69.491221999999993</v>
-      </c>
-      <c r="D3" s="34">
-        <v>1380</v>
-      </c>
-      <c r="E3" s="34">
-        <v>5</v>
-      </c>
-      <c r="F3" s="35">
-        <v>3.2</v>
-      </c>
-      <c r="G3" s="8">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="36">
-        <f>25.9*10^7</f>
-        <v>259000000</v>
-      </c>
-      <c r="K3" s="36">
-        <v>8800000</v>
+      <c r="B3" s="50">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C3" s="50">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D3" s="50">
+        <v>957</v>
+      </c>
+      <c r="E3" s="50">
+        <v>3</v>
+      </c>
+      <c r="F3" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G3" s="50">
+        <v>1</v>
+      </c>
+      <c r="H3" s="50">
+        <v>0</v>
+      </c>
+      <c r="I3" s="50">
+        <v>0</v>
+      </c>
+      <c r="J3" s="50">
+        <v>495000000</v>
+      </c>
+      <c r="K3" s="51">
+        <v>3600000</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="B4" s="8">
-        <v>-19.578942000000001</v>
-      </c>
-      <c r="C4" s="8">
-        <v>-69.872967000000003</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1172</v>
-      </c>
-      <c r="E4" s="8">
-        <v>5</v>
-      </c>
-      <c r="F4" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G4" s="8">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8">
-        <v>0</v>
-      </c>
-      <c r="J4" s="52">
-        <f>65.91*10^7</f>
-        <v>659100000</v>
-      </c>
-      <c r="K4" s="52">
-        <v>12000000</v>
+      <c r="B4" s="50">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C4" s="50">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D4" s="50">
+        <v>957</v>
+      </c>
+      <c r="E4" s="50">
+        <v>3</v>
+      </c>
+      <c r="F4" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G4" s="50">
+        <v>1</v>
+      </c>
+      <c r="H4" s="50">
+        <v>0</v>
+      </c>
+      <c r="I4" s="50">
+        <v>0</v>
+      </c>
+      <c r="J4" s="50">
+        <v>381800000</v>
+      </c>
+      <c r="K4" s="51">
+        <v>3000000</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="B5" s="8">
-        <v>-19.578942000000001</v>
-      </c>
-      <c r="C5" s="8">
-        <v>-69.872967000000003</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1172</v>
-      </c>
-      <c r="E5" s="9">
-        <v>5</v>
-      </c>
-      <c r="F5" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G5" s="8">
-        <v>1</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0</v>
-      </c>
-      <c r="J5" s="52">
-        <f>32.2*10^7</f>
-        <v>322000000</v>
-      </c>
-      <c r="K5" s="52">
-        <v>7000000</v>
+      <c r="B5" s="50">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C5" s="50">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D5" s="50">
+        <v>957</v>
+      </c>
+      <c r="E5" s="50">
+        <v>3</v>
+      </c>
+      <c r="F5" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G5" s="50">
+        <v>1</v>
+      </c>
+      <c r="H5" s="50">
+        <v>0</v>
+      </c>
+      <c r="I5" s="50">
+        <v>0</v>
+      </c>
+      <c r="J5" s="50">
+        <v>725300000</v>
+      </c>
+      <c r="K5" s="51">
+        <v>4400000</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="34">
-        <v>-19.987110999999999</v>
-      </c>
-      <c r="C6" s="34">
-        <v>-69.433610999999999</v>
-      </c>
-      <c r="D6" s="34">
-        <v>1943</v>
-      </c>
-      <c r="E6" s="34">
-        <v>5</v>
-      </c>
-      <c r="F6" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G6" s="8">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0</v>
-      </c>
-      <c r="J6" s="36">
-        <f>63.88*10^7</f>
-        <v>638800000</v>
-      </c>
-      <c r="K6" s="36">
-        <v>25700000</v>
+      <c r="B6" s="50">
+        <v>-19.541574000000001</v>
+      </c>
+      <c r="C6" s="50">
+        <v>-70.116951999999998</v>
+      </c>
+      <c r="D6" s="50">
+        <v>957</v>
+      </c>
+      <c r="E6" s="50">
+        <v>3</v>
+      </c>
+      <c r="F6" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G6" s="50">
+        <v>1</v>
+      </c>
+      <c r="H6" s="50">
+        <v>0</v>
+      </c>
+      <c r="I6" s="50">
+        <v>0</v>
+      </c>
+      <c r="J6" s="50">
+        <v>463100000</v>
+      </c>
+      <c r="K6" s="51">
+        <v>3300000</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="34">
-        <v>-19.340944</v>
-      </c>
-      <c r="C7" s="34">
-        <v>-69.727999999999994</v>
-      </c>
-      <c r="D7" s="34">
-        <v>1607</v>
-      </c>
-      <c r="E7" s="8">
-        <v>5</v>
-      </c>
-      <c r="F7" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-      <c r="J7" s="36">
-        <f>74.48*10^7</f>
-        <v>744800000</v>
-      </c>
-      <c r="K7" s="36">
-        <v>23300000</v>
+      <c r="B7" s="50">
+        <v>-19.564599999999999</v>
+      </c>
+      <c r="C7" s="50">
+        <v>-70.117283</v>
+      </c>
+      <c r="D7" s="50">
+        <v>925</v>
+      </c>
+      <c r="E7" s="50">
+        <v>3</v>
+      </c>
+      <c r="F7" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G7" s="50">
+        <v>1</v>
+      </c>
+      <c r="H7" s="50">
+        <v>0</v>
+      </c>
+      <c r="I7" s="50">
+        <v>0</v>
+      </c>
+      <c r="J7" s="50">
+        <v>501800000</v>
+      </c>
+      <c r="K7" s="51">
+        <v>3400000.0000000005</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="B8" s="34">
-        <v>-19.340944</v>
-      </c>
-      <c r="C8" s="34">
-        <v>-69.727999999999994</v>
-      </c>
-      <c r="D8" s="34">
-        <v>1607</v>
-      </c>
-      <c r="E8" s="9">
-        <v>5</v>
-      </c>
-      <c r="F8" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
-      <c r="J8" s="36">
-        <f>91.1*10^7</f>
-        <v>911000000</v>
-      </c>
-      <c r="K8" s="36">
-        <v>13000000</v>
+      <c r="B8" s="50">
+        <v>-19.564599999999999</v>
+      </c>
+      <c r="C8" s="50">
+        <v>-70.117283</v>
+      </c>
+      <c r="D8" s="50">
+        <v>925</v>
+      </c>
+      <c r="E8" s="50">
+        <v>3</v>
+      </c>
+      <c r="F8" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G8" s="50">
+        <v>1</v>
+      </c>
+      <c r="H8" s="50">
+        <v>0</v>
+      </c>
+      <c r="I8" s="50">
+        <v>0</v>
+      </c>
+      <c r="J8" s="50">
+        <v>315000000</v>
+      </c>
+      <c r="K8" s="51">
+        <v>2400000</v>
       </c>
       <c r="R8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="B9" s="34">
-        <v>-19.340944</v>
-      </c>
-      <c r="C9" s="34">
-        <v>-69.727999999999994</v>
-      </c>
-      <c r="D9" s="34">
-        <v>1607</v>
-      </c>
-      <c r="E9" s="34">
-        <v>5</v>
-      </c>
-      <c r="F9" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0</v>
-      </c>
-      <c r="J9" s="36">
-        <f>167.12*10^7</f>
-        <v>1671200000</v>
-      </c>
-      <c r="K9" s="36">
-        <v>36500000</v>
+      <c r="B9" s="50">
+        <v>-19.564599999999999</v>
+      </c>
+      <c r="C9" s="50">
+        <v>-70.117283</v>
+      </c>
+      <c r="D9" s="50">
+        <v>925</v>
+      </c>
+      <c r="E9" s="50">
+        <v>3</v>
+      </c>
+      <c r="F9" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G9" s="50">
+        <v>1</v>
+      </c>
+      <c r="H9" s="50">
+        <v>0</v>
+      </c>
+      <c r="I9" s="50">
+        <v>0</v>
+      </c>
+      <c r="J9" s="50">
+        <v>209900000.00000003</v>
+      </c>
+      <c r="K9" s="51">
+        <v>1600000</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="50" t="s">
         <v>209</v>
       </c>
-      <c r="B10" s="34">
-        <v>-19.336722000000002</v>
-      </c>
-      <c r="C10" s="34">
-        <v>-69.729611000000006</v>
-      </c>
-      <c r="D10" s="34">
-        <v>1604</v>
-      </c>
-      <c r="E10" s="8">
-        <v>5</v>
-      </c>
-      <c r="F10" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G10" s="8">
-        <v>1</v>
-      </c>
-      <c r="H10" s="8">
-        <v>0</v>
-      </c>
-      <c r="I10" s="8">
-        <v>0</v>
-      </c>
-      <c r="J10" s="36">
-        <f>24.27*10^7</f>
-        <v>242700000</v>
-      </c>
-      <c r="K10" s="36">
-        <v>10500000</v>
+      <c r="B10" s="50">
+        <v>-19.564599999999999</v>
+      </c>
+      <c r="C10" s="50">
+        <v>-70.117283</v>
+      </c>
+      <c r="D10" s="50">
+        <v>925</v>
+      </c>
+      <c r="E10" s="50">
+        <v>3</v>
+      </c>
+      <c r="F10" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G10" s="50">
+        <v>1</v>
+      </c>
+      <c r="H10" s="50">
+        <v>0</v>
+      </c>
+      <c r="I10" s="50">
+        <v>0</v>
+      </c>
+      <c r="J10" s="50">
+        <v>498800000</v>
+      </c>
+      <c r="K10" s="51">
+        <v>3100000</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="B11" s="34">
-        <v>-19.336722000000002</v>
-      </c>
-      <c r="C11" s="34">
-        <v>-69.729611000000006</v>
-      </c>
-      <c r="D11" s="34">
-        <v>1604</v>
-      </c>
-      <c r="E11" s="9">
-        <v>5</v>
-      </c>
-      <c r="F11" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G11" s="8">
-        <v>1</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="36">
-        <f>31.18*10^7</f>
-        <v>311800000</v>
-      </c>
-      <c r="K11" s="36">
-        <v>11900000</v>
+      <c r="B11" s="50">
+        <v>-19.565581999999999</v>
+      </c>
+      <c r="C11" s="50">
+        <v>-70.110219999999998</v>
+      </c>
+      <c r="D11" s="50">
+        <v>931</v>
+      </c>
+      <c r="E11" s="50">
+        <v>3</v>
+      </c>
+      <c r="F11" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G11" s="50">
+        <v>1</v>
+      </c>
+      <c r="H11" s="50">
+        <v>0</v>
+      </c>
+      <c r="I11" s="50">
+        <v>0</v>
+      </c>
+      <c r="J11" s="50">
+        <v>313400000</v>
+      </c>
+      <c r="K11" s="51">
+        <v>2000000</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="B12" s="34">
-        <v>-19.336722000000002</v>
-      </c>
-      <c r="C12" s="34">
-        <v>-69.729611000000006</v>
-      </c>
-      <c r="D12" s="34">
-        <v>1604</v>
-      </c>
-      <c r="E12" s="34">
-        <v>5</v>
-      </c>
-      <c r="F12" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G12" s="8">
-        <v>1</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8">
-        <v>0</v>
-      </c>
-      <c r="J12" s="36">
-        <f>104.68*10^7</f>
-        <v>1046800000.0000001</v>
-      </c>
-      <c r="K12" s="36">
-        <v>22400000.000000004</v>
+      <c r="B12" s="50">
+        <v>-19.565581999999999</v>
+      </c>
+      <c r="C12" s="50">
+        <v>-70.110219999999998</v>
+      </c>
+      <c r="D12" s="50">
+        <v>931</v>
+      </c>
+      <c r="E12" s="50">
+        <v>3</v>
+      </c>
+      <c r="F12" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G12" s="50">
+        <v>1</v>
+      </c>
+      <c r="H12" s="50">
+        <v>0</v>
+      </c>
+      <c r="I12" s="50">
+        <v>0</v>
+      </c>
+      <c r="J12" s="50">
+        <v>415200000.00000006</v>
+      </c>
+      <c r="K12" s="51">
+        <v>2800000.0000000005</v>
       </c>
       <c r="R12">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="B13" s="37">
-        <v>-18.886583000000002</v>
-      </c>
-      <c r="C13" s="37">
-        <v>-69.699055999999999</v>
-      </c>
-      <c r="D13" s="37">
-        <v>2282</v>
-      </c>
-      <c r="E13" s="8">
-        <v>5</v>
-      </c>
-      <c r="F13" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G13" s="8">
-        <v>1</v>
-      </c>
-      <c r="H13" s="8">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8">
-        <v>0</v>
-      </c>
-      <c r="J13" s="38">
-        <f>269.89*10^7</f>
-        <v>2698900000</v>
-      </c>
-      <c r="K13" s="38">
-        <v>47300000.000000007</v>
+      <c r="B13" s="50">
+        <v>-19.565581999999999</v>
+      </c>
+      <c r="C13" s="50">
+        <v>-70.110219999999998</v>
+      </c>
+      <c r="D13" s="50">
+        <v>931</v>
+      </c>
+      <c r="E13" s="50">
+        <v>3</v>
+      </c>
+      <c r="F13" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G13" s="50">
+        <v>1</v>
+      </c>
+      <c r="H13" s="50">
+        <v>0</v>
+      </c>
+      <c r="I13" s="50">
+        <v>0</v>
+      </c>
+      <c r="J13" s="50">
+        <v>534600000</v>
+      </c>
+      <c r="K13" s="51">
+        <v>3600000</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="B14" s="37">
-        <v>-18.886583000000002</v>
-      </c>
-      <c r="C14" s="37">
-        <v>-69.699055999999999</v>
-      </c>
-      <c r="D14" s="37">
-        <v>2282</v>
-      </c>
-      <c r="E14" s="9">
-        <v>5</v>
-      </c>
-      <c r="F14" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G14" s="8">
-        <v>1</v>
-      </c>
-      <c r="H14" s="8">
-        <v>0</v>
-      </c>
-      <c r="I14" s="8">
-        <v>0</v>
-      </c>
-      <c r="J14" s="38">
-        <f>246.53*10^7</f>
-        <v>2465300000</v>
-      </c>
-      <c r="K14" s="38">
-        <v>42900000</v>
+      <c r="B14" s="50">
+        <v>-19.565581999999999</v>
+      </c>
+      <c r="C14" s="50">
+        <v>-70.110219999999998</v>
+      </c>
+      <c r="D14" s="50">
+        <v>931</v>
+      </c>
+      <c r="E14" s="50">
+        <v>3</v>
+      </c>
+      <c r="F14" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G14" s="50">
+        <v>1</v>
+      </c>
+      <c r="H14" s="50">
+        <v>0</v>
+      </c>
+      <c r="I14" s="50">
+        <v>0</v>
+      </c>
+      <c r="J14" s="50">
+        <v>396300000</v>
+      </c>
+      <c r="K14" s="51">
+        <v>3000000</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="B15" s="37">
-        <v>-18.905639000000001</v>
-      </c>
-      <c r="C15" s="37">
-        <v>-69.954583</v>
-      </c>
-      <c r="D15" s="37">
-        <v>1443</v>
-      </c>
-      <c r="E15" s="34">
-        <v>5</v>
-      </c>
-      <c r="F15" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G15" s="8">
-        <v>1</v>
-      </c>
-      <c r="H15" s="8">
-        <v>0</v>
-      </c>
-      <c r="I15" s="8">
-        <v>0</v>
-      </c>
-      <c r="J15" s="38">
-        <v>1414100000</v>
-      </c>
-      <c r="K15" s="38">
-        <v>25200000</v>
+      <c r="B15" s="50">
+        <v>-19.551714</v>
+      </c>
+      <c r="C15" s="50">
+        <v>-70.076702999999995</v>
+      </c>
+      <c r="D15" s="50">
+        <v>1023</v>
+      </c>
+      <c r="E15" s="50">
+        <v>3</v>
+      </c>
+      <c r="F15" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G15" s="50">
+        <v>1</v>
+      </c>
+      <c r="H15" s="50">
+        <v>0</v>
+      </c>
+      <c r="I15" s="50">
+        <v>0</v>
+      </c>
+      <c r="J15" s="50">
+        <v>1799999.9999999998</v>
+      </c>
+      <c r="K15" s="51">
+        <v>700000.00000000012</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="50" t="s">
         <v>215</v>
       </c>
-      <c r="B16" s="37">
-        <v>-18.905639000000001</v>
-      </c>
-      <c r="C16" s="37">
-        <v>-69.954583</v>
-      </c>
-      <c r="D16" s="37">
-        <v>1443</v>
-      </c>
-      <c r="E16" s="8">
-        <v>5</v>
-      </c>
-      <c r="F16" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G16" s="8">
-        <v>1</v>
-      </c>
-      <c r="H16" s="8">
-        <v>0</v>
-      </c>
-      <c r="I16" s="8">
-        <v>0</v>
-      </c>
-      <c r="J16" s="38">
-        <v>1648000000</v>
-      </c>
-      <c r="K16" s="38">
-        <v>28400000</v>
+      <c r="B16" s="50">
+        <v>-19.551714</v>
+      </c>
+      <c r="C16" s="50">
+        <v>-70.076702999999995</v>
+      </c>
+      <c r="D16" s="50">
+        <v>1023</v>
+      </c>
+      <c r="E16" s="50">
+        <v>3</v>
+      </c>
+      <c r="F16" s="50">
+        <v>2.65</v>
+      </c>
+      <c r="G16" s="50">
+        <v>1</v>
+      </c>
+      <c r="H16" s="50">
+        <v>0</v>
+      </c>
+      <c r="I16" s="50">
+        <v>0</v>
+      </c>
+      <c r="J16" s="50">
+        <v>3400000.0000000005</v>
+      </c>
+      <c r="K16" s="51">
+        <v>1000000</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="B17" s="37">
-        <v>-18.852694</v>
-      </c>
-      <c r="C17" s="37">
-        <v>-69.657167000000001</v>
-      </c>
-      <c r="D17" s="37">
-        <v>2550</v>
-      </c>
-      <c r="E17" s="9">
-        <v>5</v>
-      </c>
-      <c r="F17" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G17" s="8">
-        <v>1</v>
-      </c>
-      <c r="H17" s="8">
-        <v>0</v>
-      </c>
-      <c r="I17" s="8">
-        <v>0</v>
-      </c>
-      <c r="J17" s="38">
-        <v>2350000000</v>
-      </c>
-      <c r="K17" s="38">
-        <v>40400000</v>
+      <c r="B17" s="54">
+        <v>-19.551714</v>
+      </c>
+      <c r="C17" s="54">
+        <v>-70.076702999999995</v>
+      </c>
+      <c r="D17" s="54">
+        <v>1023</v>
+      </c>
+      <c r="E17" s="50">
+        <v>3</v>
+      </c>
+      <c r="F17" s="54">
+        <v>2.65</v>
+      </c>
+      <c r="G17" s="50">
+        <v>1</v>
+      </c>
+      <c r="H17" s="50">
+        <v>0</v>
+      </c>
+      <c r="I17" s="50">
+        <v>0</v>
+      </c>
+      <c r="J17" s="54">
+        <v>2300000</v>
+      </c>
+      <c r="K17" s="55">
+        <v>400000</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
-        <v>217</v>
-      </c>
-      <c r="B18" s="37">
-        <v>-20.704083000000001</v>
-      </c>
-      <c r="C18" s="37">
-        <v>-69.420833000000002</v>
-      </c>
-      <c r="D18" s="37">
-        <v>1084</v>
-      </c>
-      <c r="E18" s="34">
-        <v>5</v>
-      </c>
-      <c r="F18" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G18" s="8">
-        <v>1</v>
-      </c>
-      <c r="H18" s="8">
-        <v>0</v>
-      </c>
-      <c r="I18" s="8">
-        <v>0</v>
-      </c>
-      <c r="J18" s="38">
-        <v>901900000</v>
-      </c>
-      <c r="K18" s="38">
-        <v>19700000</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
-        <v>218</v>
-      </c>
-      <c r="B19" s="39">
-        <v>-19.786306</v>
-      </c>
-      <c r="C19" s="39">
-        <v>-69.682000000000002</v>
-      </c>
-      <c r="D19" s="39">
-        <v>1289</v>
-      </c>
-      <c r="E19" s="8">
-        <v>5</v>
-      </c>
-      <c r="F19" s="10">
-        <v>2.89</v>
-      </c>
-      <c r="G19" s="8">
-        <v>1</v>
-      </c>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="I19" s="8">
-        <v>0</v>
-      </c>
-      <c r="J19" s="40">
-        <v>1078000000</v>
-      </c>
-      <c r="K19" s="40">
-        <v>27700000</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="B20" s="34">
-        <v>-19.786306</v>
-      </c>
-      <c r="C20" s="34">
-        <v>-69.682000000000002</v>
-      </c>
-      <c r="D20" s="34">
-        <v>1289</v>
-      </c>
-      <c r="E20" s="9">
-        <v>5</v>
-      </c>
-      <c r="F20" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G20" s="8">
-        <v>1</v>
-      </c>
-      <c r="H20" s="8">
-        <v>0</v>
-      </c>
-      <c r="I20" s="8">
-        <v>0</v>
-      </c>
-      <c r="J20" s="36">
-        <v>1024900000</v>
-      </c>
-      <c r="K20" s="36">
-        <v>24800000</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="B21" s="34">
-        <v>-19.786306</v>
-      </c>
-      <c r="C21" s="34">
-        <v>-69.682000000000002</v>
-      </c>
-      <c r="D21" s="34">
-        <v>1289</v>
-      </c>
-      <c r="E21" s="34">
-        <v>5</v>
-      </c>
-      <c r="F21" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G21" s="8">
-        <v>1</v>
-      </c>
-      <c r="H21" s="8">
-        <v>0</v>
-      </c>
-      <c r="I21" s="8">
-        <v>0</v>
-      </c>
-      <c r="J21" s="42">
-        <v>2989600000</v>
-      </c>
-      <c r="K21" s="36">
-        <v>32000000</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
+      <c r="A21" s="41"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="36"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
-        <v>221</v>
-      </c>
-      <c r="B22" s="34">
-        <v>-19.397832999999999</v>
-      </c>
-      <c r="C22" s="34">
-        <v>-69.880306000000004</v>
-      </c>
-      <c r="D22" s="34">
-        <v>1256</v>
-      </c>
-      <c r="E22" s="8">
-        <v>5</v>
-      </c>
-      <c r="F22" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G22" s="8">
-        <v>1</v>
-      </c>
-      <c r="H22" s="8">
-        <v>0</v>
-      </c>
-      <c r="I22" s="8">
-        <v>0</v>
-      </c>
-      <c r="J22" s="36">
-        <v>1942300000</v>
-      </c>
-      <c r="K22" s="36">
-        <v>46700000</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="B23" s="34">
-        <v>-19.397832999999999</v>
-      </c>
-      <c r="C23" s="34">
-        <v>-69.880306000000004</v>
-      </c>
-      <c r="D23" s="34">
-        <v>1256</v>
-      </c>
-      <c r="E23" s="9">
-        <v>5</v>
-      </c>
-      <c r="F23" s="35">
-        <v>2.74</v>
-      </c>
-      <c r="G23" s="8">
-        <v>1</v>
-      </c>
-      <c r="H23" s="8">
-        <v>0</v>
-      </c>
-      <c r="I23" s="8">
-        <v>0</v>
-      </c>
-      <c r="J23" s="36">
-        <v>3102600000</v>
-      </c>
-      <c r="K23" s="36">
-        <v>82300000</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="B24" s="34">
-        <v>-19.397832999999999</v>
-      </c>
-      <c r="C24" s="34">
-        <v>-69.880306000000004</v>
-      </c>
-      <c r="D24" s="34">
-        <v>1256</v>
-      </c>
-      <c r="E24" s="34">
-        <v>5</v>
-      </c>
-      <c r="F24" s="43">
-        <v>2.89</v>
-      </c>
-      <c r="G24" s="8">
-        <v>1</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0</v>
-      </c>
-      <c r="I24" s="8">
-        <v>0</v>
-      </c>
-      <c r="J24" s="36">
-        <v>2691600000.0000005</v>
-      </c>
-      <c r="K24" s="36">
-        <v>61800000</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="B25" s="37">
-        <v>-19.522110999999999</v>
-      </c>
-      <c r="C25" s="37">
-        <v>-69.808333000000005</v>
-      </c>
-      <c r="D25" s="37">
-        <v>1312</v>
-      </c>
-      <c r="E25" s="8">
-        <v>5</v>
-      </c>
-      <c r="F25" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G25" s="8">
-        <v>1</v>
-      </c>
-      <c r="H25" s="8">
-        <v>0</v>
-      </c>
-      <c r="I25" s="8">
-        <v>0</v>
-      </c>
-      <c r="J25" s="38">
-        <v>2771500000</v>
-      </c>
-      <c r="K25" s="38">
-        <v>52000000</v>
-      </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="37" t="s">
-        <v>225</v>
-      </c>
-      <c r="B26" s="37">
-        <v>-19.522110999999999</v>
-      </c>
-      <c r="C26" s="37">
-        <v>-69.808333000000005</v>
-      </c>
-      <c r="D26" s="37">
-        <v>1312</v>
-      </c>
-      <c r="E26" s="9">
-        <v>5</v>
-      </c>
-      <c r="F26" s="35">
-        <v>2.89</v>
-      </c>
-      <c r="G26" s="8">
-        <v>1</v>
-      </c>
-      <c r="H26" s="8">
-        <v>0</v>
-      </c>
-      <c r="I26" s="8">
-        <v>0</v>
-      </c>
-      <c r="J26" s="38">
-        <v>654000000</v>
-      </c>
-      <c r="K26" s="38">
-        <v>15000000</v>
-      </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="B27" s="45">
-        <v>-18.503527999999999</v>
-      </c>
-      <c r="C27" s="45">
-        <v>-70.143305999999995</v>
-      </c>
-      <c r="D27" s="45">
-        <v>771</v>
-      </c>
-      <c r="E27" s="34">
-        <v>5</v>
-      </c>
-      <c r="F27" s="46">
-        <v>2.89</v>
-      </c>
-      <c r="G27" s="8">
-        <v>1</v>
-      </c>
-      <c r="H27" s="8">
-        <v>0</v>
-      </c>
-      <c r="I27" s="8">
-        <v>0</v>
-      </c>
-      <c r="J27" s="47">
-        <v>412900000</v>
-      </c>
-      <c r="K27" s="47">
-        <v>7200000</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
+      <c r="A27" s="44"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="48" t="s">
-        <v>227</v>
-      </c>
-      <c r="B28" s="48">
-        <v>-18.389944</v>
-      </c>
-      <c r="C28" s="48">
-        <v>-70.071805999999995</v>
-      </c>
-      <c r="D28" s="48">
-        <v>1025</v>
-      </c>
-      <c r="E28" s="8">
-        <v>5</v>
-      </c>
-      <c r="F28" s="10">
-        <v>2.89</v>
-      </c>
-      <c r="G28" s="8">
-        <v>1</v>
-      </c>
-      <c r="H28" s="8">
-        <v>0</v>
-      </c>
-      <c r="I28" s="8">
-        <v>0</v>
-      </c>
-      <c r="J28" s="49">
-        <v>388000000</v>
-      </c>
-      <c r="K28" s="49">
-        <v>7700000</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
+      <c r="A28" s="48"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="45" t="s">
-        <v>228</v>
-      </c>
-      <c r="B29" s="45">
-        <v>-18.389944</v>
-      </c>
-      <c r="C29" s="45">
-        <v>-70.071805999999995</v>
-      </c>
-      <c r="D29" s="45">
-        <v>1025</v>
-      </c>
-      <c r="E29" s="9">
-        <v>5</v>
-      </c>
-      <c r="F29" s="46">
-        <v>2.89</v>
-      </c>
-      <c r="G29" s="8">
-        <v>1</v>
-      </c>
-      <c r="H29" s="8">
-        <v>0</v>
-      </c>
-      <c r="I29" s="8">
-        <v>0</v>
-      </c>
-      <c r="J29" s="47">
-        <v>425000000</v>
-      </c>
-      <c r="K29" s="47">
-        <v>9500000</v>
-      </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
+      <c r="A29" s="45"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E30" s="1"/>
@@ -9067,37 +8735,37 @@
       <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="60" t="s">
+      <c r="F15" s="61" t="s">
         <v>25</v>
       </c>
       <c r="G15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="63" t="s">
+      <c r="H15" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="64" t="s">
+      <c r="I15" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="J15" s="55" t="s">
+      <c r="J15" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="K15" s="55" t="s">
+      <c r="K15" s="66" t="s">
         <v>29</v>
       </c>
       <c r="M15" s="21" t="s">
@@ -9123,19 +8791,19 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61" t="s">
+      <c r="A16" s="60"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="63"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
       <c r="M16" s="22" t="s">
         <v>32</v>
       </c>
@@ -9147,22 +8815,22 @@
       <c r="Q16" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="S16" s="54" t="s">
+      <c r="S16" s="60" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
       <c r="M17" s="22" t="s">
         <v>33</v>
       </c>
@@ -9178,20 +8846,20 @@
       <c r="Q17" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="S17" s="54"/>
+      <c r="S17" s="60"/>
     </row>
     <row r="18" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
       <c r="M18" s="23" t="s">
         <v>34</v>
       </c>
@@ -9200,36 +8868,36 @@
       <c r="Q18" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="S18" s="54"/>
+      <c r="S18" s="60"/>
     </row>
     <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="G19" s="62"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="55"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
       <c r="O19" s="57"/>
       <c r="P19" s="59"/>
       <c r="Q19" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="S19" s="54"/>
+      <c r="S19" s="60"/>
     </row>
     <row r="20" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="H20" s="29"/>
       <c r="I20" s="28"/>
-      <c r="P20" s="65" t="s">
+      <c r="P20" s="67" t="s">
         <v>52</v>
       </c>
       <c r="Q20" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="S20" s="54"/>
+      <c r="S20" s="60"/>
     </row>
     <row r="21" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
-      <c r="P21" s="66"/>
+      <c r="P21" s="68"/>
       <c r="Q21" s="30" t="s">
         <v>43</v>
       </c>
@@ -9237,7 +8905,7 @@
     <row r="22" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
-      <c r="P22" s="66"/>
+      <c r="P22" s="68"/>
       <c r="Q22" s="31" t="s">
         <v>44</v>
       </c>
@@ -9245,33 +8913,38 @@
     <row r="23" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
-      <c r="P23" s="66"/>
+      <c r="P23" s="68"/>
     </row>
     <row r="24" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
-      <c r="P24" s="66"/>
+      <c r="P24" s="68"/>
     </row>
     <row r="25" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
-      <c r="P25" s="66"/>
+      <c r="P25" s="68"/>
     </row>
     <row r="26" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
-      <c r="P26" s="66"/>
+      <c r="P26" s="68"/>
     </row>
     <row r="27" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
-      <c r="P27" s="66"/>
+      <c r="P27" s="68"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P28" s="67"/>
+      <c r="P28" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="K15:K19"/>
     <mergeCell ref="O17:O19"/>
     <mergeCell ref="P17:P19"/>
     <mergeCell ref="S16:S20"/>
@@ -9282,11 +8955,6 @@
     <mergeCell ref="J15:J19"/>
     <mergeCell ref="P20:P28"/>
     <mergeCell ref="I15:I19"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="K15:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>